<commit_message>
updating the Software steps pdf to include steps to get the android app, and reorganized a bit of the sections in this document
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -1550,7 +1550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1998,11 +1998,14 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2286,9 +2289,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA970"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L89" sqref="L89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -2444,7 +2447,7 @@
         <v>44</v>
       </c>
       <c r="M3" s="44"/>
-      <c r="N3" s="163" t="s">
+      <c r="N3" s="164" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2485,7 +2488,7 @@
         <v>49</v>
       </c>
       <c r="M4" s="48"/>
-      <c r="N4" s="164"/>
+      <c r="N4" s="165"/>
       <c r="Y4" s="49"/>
       <c r="Z4" s="49"/>
       <c r="AA4" s="49"/>
@@ -5849,7 +5852,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L89" s="85" t="s">
+      <c r="L89" s="166" t="s">
         <v>319</v>
       </c>
     </row>
@@ -6405,7 +6408,7 @@
       <c r="F105" s="141" t="s">
         <v>380</v>
       </c>
-      <c r="G105" s="165"/>
+      <c r="G105" s="163"/>
       <c r="H105" s="143" t="s">
         <v>67</v>
       </c>
@@ -6439,7 +6442,7 @@
       <c r="F106" s="141" t="s">
         <v>197</v>
       </c>
-      <c r="G106" s="165"/>
+      <c r="G106" s="163"/>
       <c r="H106" s="143" t="s">
         <v>67</v>
       </c>
@@ -18644,9 +18647,10 @@
     <hyperlink ref="L43" r:id="rId86" location="92141A008"/>
     <hyperlink ref="L105" r:id="rId87"/>
     <hyperlink ref="L106" r:id="rId88"/>
+    <hyperlink ref="L89" r:id="rId89"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId89"/>
+  <pageSetup orientation="portrait" r:id="rId90"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added a specs feature to top level readme
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="388">
   <si>
     <t>Part</t>
   </si>
@@ -1189,6 +1189,9 @@
   </si>
   <si>
     <t>© 2018 California Institute of Technology. Government sponsorship acknowledged</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/category/115/25d-mm-metal-gearmotors</t>
   </si>
 </sst>
 </file>
@@ -2013,10 +2016,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2024,14 +2023,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2040,6 +2040,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2324,9 +2327,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA970"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A1:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -2349,52 +2352,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="167" customFormat="1" ht="32.65" customHeight="1">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="176" t="s">
         <v>384</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="179"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
     </row>
     <row r="2" spans="1:27" s="169" customFormat="1" ht="27.4" customHeight="1">
-      <c r="A2" s="174" t="s">
+      <c r="A2" s="179" t="s">
         <v>385</v>
       </c>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="175"/>
-      <c r="L2" s="175"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
     </row>
     <row r="3" spans="1:27" s="169" customFormat="1" ht="27" customHeight="1">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="173" t="s">
         <v>386</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="172"/>
-      <c r="H3" s="172"/>
-      <c r="I3" s="173"/>
-      <c r="J3" s="172"/>
-      <c r="K3" s="172"/>
-      <c r="L3" s="172"/>
+      <c r="B3" s="173"/>
+      <c r="C3" s="173"/>
+      <c r="D3" s="173"/>
+      <c r="E3" s="173"/>
+      <c r="F3" s="173"/>
+      <c r="G3" s="170"/>
+      <c r="H3" s="170"/>
+      <c r="I3" s="171"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
     </row>
     <row r="4" spans="1:27" ht="45" customHeight="1">
       <c r="A4" s="27" t="s">
@@ -2530,7 +2533,7 @@
         <v>44</v>
       </c>
       <c r="M6" s="39"/>
-      <c r="N6" s="170" t="s">
+      <c r="N6" s="174" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2571,7 +2574,7 @@
         <v>49</v>
       </c>
       <c r="M7" s="40"/>
-      <c r="N7" s="171"/>
+      <c r="N7" s="175"/>
       <c r="Y7" s="41"/>
       <c r="Z7" s="41"/>
       <c r="AA7" s="41"/>
@@ -4300,7 +4303,7 @@
         <v>209.70000000000002</v>
       </c>
       <c r="L50" s="86" t="s">
-        <v>199</v>
+        <v>387</v>
       </c>
       <c r="M50" s="34"/>
     </row>
@@ -15978,72 +15981,71 @@
     <hyperlink ref="L46" r:id="rId19" location="92141A005"/>
     <hyperlink ref="L48" r:id="rId20"/>
     <hyperlink ref="L49" r:id="rId21"/>
-    <hyperlink ref="L50" r:id="rId22"/>
-    <hyperlink ref="L51" r:id="rId23"/>
-    <hyperlink ref="L52" r:id="rId24"/>
-    <hyperlink ref="L53" r:id="rId25"/>
-    <hyperlink ref="L54" r:id="rId26"/>
-    <hyperlink ref="L55" r:id="rId27" location="348=95"/>
-    <hyperlink ref="L56" r:id="rId28" location="348=107"/>
-    <hyperlink ref="L57" r:id="rId29" location="348=96"/>
-    <hyperlink ref="L58" r:id="rId30" location="371=276"/>
-    <hyperlink ref="L59" r:id="rId31"/>
-    <hyperlink ref="L60" r:id="rId32" location="371=455"/>
-    <hyperlink ref="L61" r:id="rId33" location="371=246"/>
-    <hyperlink ref="L62" r:id="rId34"/>
-    <hyperlink ref="L63" r:id="rId35"/>
-    <hyperlink ref="L64" r:id="rId36"/>
-    <hyperlink ref="L65" r:id="rId37" location="348=123"/>
-    <hyperlink ref="L66" r:id="rId38"/>
-    <hyperlink ref="L67" r:id="rId39"/>
-    <hyperlink ref="L68" r:id="rId40" location="199=15"/>
-    <hyperlink ref="L69" r:id="rId41"/>
-    <hyperlink ref="L70" r:id="rId42"/>
-    <hyperlink ref="L71" r:id="rId43"/>
-    <hyperlink ref="L72" r:id="rId44"/>
-    <hyperlink ref="L74" r:id="rId45"/>
-    <hyperlink ref="L75" r:id="rId46"/>
-    <hyperlink ref="L76" r:id="rId47"/>
-    <hyperlink ref="L77" r:id="rId48"/>
-    <hyperlink ref="L78" r:id="rId49"/>
-    <hyperlink ref="L79" r:id="rId50" location="371=256"/>
-    <hyperlink ref="L80" r:id="rId51"/>
-    <hyperlink ref="L81" r:id="rId52"/>
-    <hyperlink ref="L82" r:id="rId53"/>
-    <hyperlink ref="L88" r:id="rId54"/>
-    <hyperlink ref="L89" r:id="rId55"/>
-    <hyperlink ref="L92" r:id="rId56"/>
-    <hyperlink ref="L93" r:id="rId57"/>
-    <hyperlink ref="L94" r:id="rId58"/>
-    <hyperlink ref="L95" r:id="rId59"/>
-    <hyperlink ref="L96" r:id="rId60"/>
-    <hyperlink ref="L98" r:id="rId61"/>
-    <hyperlink ref="L100" r:id="rId62"/>
-    <hyperlink ref="L101" r:id="rId63"/>
-    <hyperlink ref="L102" r:id="rId64"/>
-    <hyperlink ref="L73" r:id="rId65"/>
-    <hyperlink ref="L24" r:id="rId66" location="92949a144/=18njs1n"/>
-    <hyperlink ref="L30" r:id="rId67" location="92949A150"/>
-    <hyperlink ref="L34" r:id="rId68" location="92949a106/=18njrx6"/>
-    <hyperlink ref="L104" r:id="rId69" location="93330A252"/>
-    <hyperlink ref="L27" r:id="rId70" location="90631A005"/>
-    <hyperlink ref="L28" r:id="rId71" location="92949A146"/>
-    <hyperlink ref="L29" r:id="rId72" location="92949A148"/>
-    <hyperlink ref="L31" r:id="rId73" location="92949A151"/>
-    <hyperlink ref="L32" r:id="rId74" location="92949A153"/>
-    <hyperlink ref="L33" r:id="rId75" location="92949A160"/>
-    <hyperlink ref="L39" r:id="rId76" location="92510A442"/>
-    <hyperlink ref="L41" r:id="rId77" location="91780A162"/>
-    <hyperlink ref="L42" r:id="rId78" location="91780A164"/>
-    <hyperlink ref="L43" r:id="rId79" location="91780A166"/>
-    <hyperlink ref="L47" r:id="rId80" location="91545A280"/>
-    <hyperlink ref="L45" r:id="rId81" location="92141A008"/>
-    <hyperlink ref="L105" r:id="rId82"/>
-    <hyperlink ref="L106" r:id="rId83"/>
-    <hyperlink ref="L91" r:id="rId84"/>
+    <hyperlink ref="L51" r:id="rId22"/>
+    <hyperlink ref="L52" r:id="rId23"/>
+    <hyperlink ref="L53" r:id="rId24"/>
+    <hyperlink ref="L54" r:id="rId25"/>
+    <hyperlink ref="L55" r:id="rId26" location="348=95"/>
+    <hyperlink ref="L56" r:id="rId27" location="348=107"/>
+    <hyperlink ref="L57" r:id="rId28" location="348=96"/>
+    <hyperlink ref="L58" r:id="rId29" location="371=276"/>
+    <hyperlink ref="L59" r:id="rId30"/>
+    <hyperlink ref="L60" r:id="rId31" location="371=455"/>
+    <hyperlink ref="L61" r:id="rId32" location="371=246"/>
+    <hyperlink ref="L62" r:id="rId33"/>
+    <hyperlink ref="L63" r:id="rId34"/>
+    <hyperlink ref="L64" r:id="rId35"/>
+    <hyperlink ref="L65" r:id="rId36" location="348=123"/>
+    <hyperlink ref="L66" r:id="rId37"/>
+    <hyperlink ref="L67" r:id="rId38"/>
+    <hyperlink ref="L68" r:id="rId39" location="199=15"/>
+    <hyperlink ref="L69" r:id="rId40"/>
+    <hyperlink ref="L70" r:id="rId41"/>
+    <hyperlink ref="L71" r:id="rId42"/>
+    <hyperlink ref="L72" r:id="rId43"/>
+    <hyperlink ref="L74" r:id="rId44"/>
+    <hyperlink ref="L75" r:id="rId45"/>
+    <hyperlink ref="L76" r:id="rId46"/>
+    <hyperlink ref="L77" r:id="rId47"/>
+    <hyperlink ref="L78" r:id="rId48"/>
+    <hyperlink ref="L79" r:id="rId49" location="371=256"/>
+    <hyperlink ref="L80" r:id="rId50"/>
+    <hyperlink ref="L81" r:id="rId51"/>
+    <hyperlink ref="L82" r:id="rId52"/>
+    <hyperlink ref="L88" r:id="rId53"/>
+    <hyperlink ref="L89" r:id="rId54"/>
+    <hyperlink ref="L92" r:id="rId55"/>
+    <hyperlink ref="L93" r:id="rId56"/>
+    <hyperlink ref="L94" r:id="rId57"/>
+    <hyperlink ref="L95" r:id="rId58"/>
+    <hyperlink ref="L96" r:id="rId59"/>
+    <hyperlink ref="L98" r:id="rId60"/>
+    <hyperlink ref="L100" r:id="rId61"/>
+    <hyperlink ref="L101" r:id="rId62"/>
+    <hyperlink ref="L102" r:id="rId63"/>
+    <hyperlink ref="L73" r:id="rId64"/>
+    <hyperlink ref="L24" r:id="rId65" location="92949a144/=18njs1n"/>
+    <hyperlink ref="L30" r:id="rId66" location="92949A150"/>
+    <hyperlink ref="L34" r:id="rId67" location="92949a106/=18njrx6"/>
+    <hyperlink ref="L104" r:id="rId68" location="93330A252"/>
+    <hyperlink ref="L27" r:id="rId69" location="90631A005"/>
+    <hyperlink ref="L28" r:id="rId70" location="92949A146"/>
+    <hyperlink ref="L29" r:id="rId71" location="92949A148"/>
+    <hyperlink ref="L31" r:id="rId72" location="92949A151"/>
+    <hyperlink ref="L32" r:id="rId73" location="92949A153"/>
+    <hyperlink ref="L33" r:id="rId74" location="92949A160"/>
+    <hyperlink ref="L39" r:id="rId75" location="92510A442"/>
+    <hyperlink ref="L41" r:id="rId76" location="91780A162"/>
+    <hyperlink ref="L42" r:id="rId77" location="91780A164"/>
+    <hyperlink ref="L43" r:id="rId78" location="91780A166"/>
+    <hyperlink ref="L47" r:id="rId79" location="91545A280"/>
+    <hyperlink ref="L45" r:id="rId80" location="92141A008"/>
+    <hyperlink ref="L105" r:id="rId81"/>
+    <hyperlink ref="L106" r:id="rId82"/>
+    <hyperlink ref="L91" r:id="rId83"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId85"/>
+  <pageSetup orientation="portrait" r:id="rId84"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updating README.md to have parts list wishlists
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -2325,11 +2325,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA970"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L89" sqref="L89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
@@ -2452,7 +2453,7 @@
       <c r="Z4" s="29"/>
       <c r="AA4" s="29"/>
     </row>
-    <row r="5" spans="1:27" ht="14.25" customHeight="1">
+    <row r="5" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A5" s="111" t="s">
         <v>38</v>
       </c>
@@ -2496,7 +2497,7 @@
       <c r="Z5" s="34"/>
       <c r="AA5" s="34"/>
     </row>
-    <row r="6" spans="1:27" ht="14.25" customHeight="1">
+    <row r="6" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A6" s="79" t="s">
         <v>41</v>
       </c>
@@ -2537,7 +2538,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1">
+    <row r="7" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A7" s="120" t="s">
         <v>46</v>
       </c>
@@ -2579,7 +2580,7 @@
       <c r="Z7" s="41"/>
       <c r="AA7" s="41"/>
     </row>
-    <row r="8" spans="1:27" ht="14.25" customHeight="1">
+    <row r="8" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A8" s="79" t="s">
         <v>50</v>
       </c>
@@ -2617,7 +2618,7 @@
       </c>
       <c r="M8" s="34"/>
     </row>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1">
+    <row r="9" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A9" s="79" t="s">
         <v>52</v>
       </c>
@@ -2655,7 +2656,7 @@
       </c>
       <c r="M9" s="34"/>
     </row>
-    <row r="10" spans="1:27" s="95" customFormat="1" ht="14.25" customHeight="1">
+    <row r="10" spans="1:27" s="95" customFormat="1" ht="14.25" hidden="1" customHeight="1">
       <c r="A10" s="120" t="s">
         <v>56</v>
       </c>
@@ -2696,7 +2697,7 @@
       <c r="Z10" s="96"/>
       <c r="AA10" s="96"/>
     </row>
-    <row r="11" spans="1:27" ht="14.25">
+    <row r="11" spans="1:27" ht="14.25" hidden="1">
       <c r="A11" s="87" t="s">
         <v>59</v>
       </c>
@@ -2734,7 +2735,7 @@
       </c>
       <c r="M11" s="34"/>
     </row>
-    <row r="12" spans="1:27" ht="14.25">
+    <row r="12" spans="1:27" ht="14.25" hidden="1">
       <c r="A12" s="79" t="s">
         <v>62</v>
       </c>
@@ -2774,7 +2775,7 @@
       </c>
       <c r="M12" s="46"/>
     </row>
-    <row r="13" spans="1:27" ht="14.25">
+    <row r="13" spans="1:27" ht="14.25" hidden="1">
       <c r="A13" s="79" t="s">
         <v>67</v>
       </c>
@@ -2815,7 +2816,7 @@
       <c r="Z13" s="41"/>
       <c r="AA13" s="41"/>
     </row>
-    <row r="14" spans="1:27" ht="14.25">
+    <row r="14" spans="1:27" ht="14.25" hidden="1">
       <c r="A14" s="79" t="s">
         <v>71</v>
       </c>
@@ -2853,7 +2854,7 @@
       </c>
       <c r="M14" s="34"/>
     </row>
-    <row r="15" spans="1:27" ht="28.5">
+    <row r="15" spans="1:27" ht="28.5" hidden="1">
       <c r="A15" s="79" t="s">
         <v>74</v>
       </c>
@@ -2891,7 +2892,7 @@
       </c>
       <c r="M15" s="34"/>
     </row>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1">
+    <row r="16" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A16" s="79" t="s">
         <v>79</v>
       </c>
@@ -2962,7 +2963,7 @@
         <f t="shared" si="1"/>
         <v>0.70000000000000007</v>
       </c>
-      <c r="L17" s="85" t="s">
+      <c r="L17" s="168" t="s">
         <v>368</v>
       </c>
       <c r="M17" s="34"/>
@@ -3000,7 +3001,7 @@
         <f t="shared" si="1"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="L18" s="86" t="s">
+      <c r="L18" s="168" t="s">
         <v>369</v>
       </c>
       <c r="M18" s="34"/>
@@ -3081,7 +3082,7 @@
       </c>
       <c r="M20" s="34"/>
     </row>
-    <row r="21" spans="1:27" ht="14.25" customHeight="1">
+    <row r="21" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A21" s="79" t="s">
         <v>89</v>
       </c>
@@ -3121,7 +3122,7 @@
       </c>
       <c r="M21" s="34"/>
     </row>
-    <row r="22" spans="1:27" ht="14.25" customHeight="1">
+    <row r="22" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A22" s="79" t="s">
         <v>93</v>
       </c>
@@ -3161,7 +3162,7 @@
       </c>
       <c r="M22" s="34"/>
     </row>
-    <row r="23" spans="1:27" ht="14.25" customHeight="1">
+    <row r="23" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A23" s="79" t="s">
         <v>97</v>
       </c>
@@ -3202,7 +3203,7 @@
       </c>
       <c r="M23" s="34"/>
     </row>
-    <row r="24" spans="1:27" ht="14.25" customHeight="1">
+    <row r="24" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A24" s="79" t="s">
         <v>346</v>
       </c>
@@ -3243,7 +3244,7 @@
       </c>
       <c r="M24" s="34"/>
     </row>
-    <row r="25" spans="1:27" ht="14.25" customHeight="1">
+    <row r="25" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A25" s="79" t="s">
         <v>105</v>
       </c>
@@ -3287,7 +3288,7 @@
       <c r="Z25" s="34"/>
       <c r="AA25" s="34"/>
     </row>
-    <row r="26" spans="1:27" ht="14.25" customHeight="1">
+    <row r="26" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A26" s="79" t="s">
         <v>108</v>
       </c>
@@ -3330,7 +3331,7 @@
       <c r="Z26" s="34"/>
       <c r="AA26" s="34"/>
     </row>
-    <row r="27" spans="1:27" ht="14.25" customHeight="1">
+    <row r="27" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A27" s="79" t="s">
         <v>112</v>
       </c>
@@ -3373,7 +3374,7 @@
       <c r="Z27" s="34"/>
       <c r="AA27" s="34"/>
     </row>
-    <row r="28" spans="1:27" ht="14.25" customHeight="1">
+    <row r="28" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A28" s="79" t="s">
         <v>349</v>
       </c>
@@ -3417,7 +3418,7 @@
       <c r="Z28" s="34"/>
       <c r="AA28" s="34"/>
     </row>
-    <row r="29" spans="1:27" ht="14.25" customHeight="1">
+    <row r="29" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A29" s="79" t="s">
         <v>350</v>
       </c>
@@ -3460,7 +3461,7 @@
       <c r="Z29" s="34"/>
       <c r="AA29" s="34"/>
     </row>
-    <row r="30" spans="1:27" ht="14.25" customHeight="1">
+    <row r="30" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A30" s="79" t="s">
         <v>353</v>
       </c>
@@ -3500,7 +3501,7 @@
       </c>
       <c r="M30" s="34"/>
     </row>
-    <row r="31" spans="1:27" ht="14.25" customHeight="1">
+    <row r="31" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A31" s="79" t="s">
         <v>354</v>
       </c>
@@ -3540,7 +3541,7 @@
       </c>
       <c r="M31" s="34"/>
     </row>
-    <row r="32" spans="1:27" ht="14.25" customHeight="1">
+    <row r="32" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A32" s="79" t="s">
         <v>356</v>
       </c>
@@ -3580,7 +3581,7 @@
       </c>
       <c r="M32" s="34"/>
     </row>
-    <row r="33" spans="1:27" ht="14.25" customHeight="1">
+    <row r="33" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A33" s="79" t="s">
         <v>358</v>
       </c>
@@ -3620,7 +3621,7 @@
       </c>
       <c r="M33" s="34"/>
     </row>
-    <row r="34" spans="1:27" ht="14.25" customHeight="1">
+    <row r="34" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A34" s="79" t="s">
         <v>359</v>
       </c>
@@ -3660,7 +3661,7 @@
       </c>
       <c r="M34" s="34"/>
     </row>
-    <row r="35" spans="1:27" ht="14.25" customHeight="1">
+    <row r="35" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A35" s="79" t="s">
         <v>360</v>
       </c>
@@ -3700,7 +3701,7 @@
       </c>
       <c r="M35" s="34"/>
     </row>
-    <row r="36" spans="1:27" ht="14.25" customHeight="1">
+    <row r="36" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A36" s="79" t="s">
         <v>145</v>
       </c>
@@ -3740,7 +3741,7 @@
       </c>
       <c r="M36" s="34"/>
     </row>
-    <row r="37" spans="1:27" ht="14.25" customHeight="1">
+    <row r="37" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A37" s="79" t="s">
         <v>147</v>
       </c>
@@ -3780,7 +3781,7 @@
       </c>
       <c r="M37" s="34"/>
     </row>
-    <row r="38" spans="1:27" ht="14.25" customHeight="1">
+    <row r="38" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A38" s="79" t="s">
         <v>151</v>
       </c>
@@ -3820,7 +3821,7 @@
       </c>
       <c r="M38" s="34"/>
     </row>
-    <row r="39" spans="1:27" ht="14.25" customHeight="1">
+    <row r="39" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A39" s="79" t="s">
         <v>155</v>
       </c>
@@ -3860,7 +3861,7 @@
       </c>
       <c r="M39" s="34"/>
     </row>
-    <row r="40" spans="1:27" ht="14.25" customHeight="1">
+    <row r="40" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A40" s="79" t="s">
         <v>159</v>
       </c>
@@ -3901,7 +3902,7 @@
       </c>
       <c r="M40" s="34"/>
     </row>
-    <row r="41" spans="1:27" ht="14.25" customHeight="1">
+    <row r="41" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A41" s="79" t="s">
         <v>162</v>
       </c>
@@ -3941,7 +3942,7 @@
       </c>
       <c r="M41" s="34"/>
     </row>
-    <row r="42" spans="1:27" ht="14.25" customHeight="1">
+    <row r="42" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A42" s="79" t="s">
         <v>166</v>
       </c>
@@ -3984,7 +3985,7 @@
       <c r="Z42" s="34"/>
       <c r="AA42" s="34"/>
     </row>
-    <row r="43" spans="1:27" ht="14.25" customHeight="1">
+    <row r="43" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A43" s="79" t="s">
         <v>170</v>
       </c>
@@ -4027,7 +4028,7 @@
       <c r="Z43" s="34"/>
       <c r="AA43" s="34"/>
     </row>
-    <row r="44" spans="1:27" ht="14.25" customHeight="1">
+    <row r="44" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A44" s="79" t="s">
         <v>174</v>
       </c>
@@ -4070,7 +4071,7 @@
       <c r="Z44" s="34"/>
       <c r="AA44" s="34"/>
     </row>
-    <row r="45" spans="1:27" ht="14.25" customHeight="1">
+    <row r="45" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A45" s="79" t="s">
         <v>178</v>
       </c>
@@ -4113,7 +4114,7 @@
       <c r="Z45" s="34"/>
       <c r="AA45" s="34"/>
     </row>
-    <row r="46" spans="1:27" ht="14.25" customHeight="1">
+    <row r="46" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A46" s="79" t="s">
         <v>182</v>
       </c>
@@ -4153,7 +4154,7 @@
       </c>
       <c r="M46" s="34"/>
     </row>
-    <row r="47" spans="1:27" ht="14.25" customHeight="1">
+    <row r="47" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A47" s="79" t="s">
         <v>186</v>
       </c>
@@ -4193,7 +4194,7 @@
       </c>
       <c r="M47" s="34"/>
     </row>
-    <row r="48" spans="1:27" ht="14.25" customHeight="1">
+    <row r="48" spans="1:27" ht="14.25" hidden="1" customHeight="1">
       <c r="A48" s="79" t="s">
         <v>194</v>
       </c>
@@ -4231,7 +4232,7 @@
       </c>
       <c r="M48" s="34"/>
     </row>
-    <row r="49" spans="1:13" ht="14.25" customHeight="1">
+    <row r="49" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A49" s="79" t="s">
         <v>196</v>
       </c>
@@ -4269,7 +4270,7 @@
       </c>
       <c r="M49" s="34"/>
     </row>
-    <row r="50" spans="1:13" ht="14.25" customHeight="1">
+    <row r="50" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A50" s="79" t="s">
         <v>198</v>
       </c>
@@ -4307,7 +4308,7 @@
       </c>
       <c r="M50" s="34"/>
     </row>
-    <row r="51" spans="1:13" ht="14.25" customHeight="1">
+    <row r="51" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A51" s="79" t="s">
         <v>200</v>
       </c>
@@ -4345,7 +4346,7 @@
       </c>
       <c r="M51" s="34"/>
     </row>
-    <row r="52" spans="1:13" ht="14.25" customHeight="1">
+    <row r="52" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A52" s="79" t="s">
         <v>203</v>
       </c>
@@ -4385,7 +4386,7 @@
       </c>
       <c r="M52" s="34"/>
     </row>
-    <row r="53" spans="1:13" ht="14.25" customHeight="1">
+    <row r="53" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A53" s="79" t="s">
         <v>206</v>
       </c>
@@ -4425,7 +4426,7 @@
       </c>
       <c r="M53" s="34"/>
     </row>
-    <row r="54" spans="1:13" ht="14.25" customHeight="1">
+    <row r="54" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A54" s="79" t="s">
         <v>209</v>
       </c>
@@ -4465,7 +4466,7 @@
       </c>
       <c r="M54" s="34"/>
     </row>
-    <row r="55" spans="1:13" ht="14.25" customHeight="1">
+    <row r="55" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A55" s="79" t="s">
         <v>212</v>
       </c>
@@ -4505,7 +4506,7 @@
       </c>
       <c r="M55" s="34"/>
     </row>
-    <row r="56" spans="1:13" ht="14.25" customHeight="1">
+    <row r="56" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A56" s="79" t="s">
         <v>215</v>
       </c>
@@ -4545,7 +4546,7 @@
       </c>
       <c r="M56" s="34"/>
     </row>
-    <row r="57" spans="1:13" ht="14.25" customHeight="1">
+    <row r="57" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A57" s="79" t="s">
         <v>218</v>
       </c>
@@ -4585,7 +4586,7 @@
       </c>
       <c r="M57" s="34"/>
     </row>
-    <row r="58" spans="1:13" ht="14.25" customHeight="1">
+    <row r="58" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A58" s="79" t="s">
         <v>220</v>
       </c>
@@ -4625,7 +4626,7 @@
       </c>
       <c r="M58" s="34"/>
     </row>
-    <row r="59" spans="1:13" ht="14.25" customHeight="1">
+    <row r="59" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A59" s="79" t="s">
         <v>223</v>
       </c>
@@ -4663,7 +4664,7 @@
       </c>
       <c r="M59" s="34"/>
     </row>
-    <row r="60" spans="1:13" ht="14.25" customHeight="1">
+    <row r="60" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A60" s="87" t="s">
         <v>226</v>
       </c>
@@ -4703,7 +4704,7 @@
       </c>
       <c r="M60" s="34"/>
     </row>
-    <row r="61" spans="1:13" ht="14.25" customHeight="1">
+    <row r="61" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A61" s="87" t="s">
         <v>229</v>
       </c>
@@ -4743,7 +4744,7 @@
       </c>
       <c r="M61" s="34"/>
     </row>
-    <row r="62" spans="1:13" ht="14.25" customHeight="1">
+    <row r="62" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A62" s="79" t="s">
         <v>232</v>
       </c>
@@ -4783,7 +4784,7 @@
       </c>
       <c r="M62" s="34"/>
     </row>
-    <row r="63" spans="1:13" ht="14.25" customHeight="1">
+    <row r="63" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A63" s="79" t="s">
         <v>235</v>
       </c>
@@ -4823,7 +4824,7 @@
       </c>
       <c r="M63" s="34"/>
     </row>
-    <row r="64" spans="1:13" ht="14.25" customHeight="1">
+    <row r="64" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A64" s="79" t="s">
         <v>237</v>
       </c>
@@ -4863,7 +4864,7 @@
       </c>
       <c r="M64" s="34"/>
     </row>
-    <row r="65" spans="1:13" ht="14.25" customHeight="1">
+    <row r="65" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A65" s="79" t="s">
         <v>240</v>
       </c>
@@ -4903,7 +4904,7 @@
       </c>
       <c r="M65" s="34"/>
     </row>
-    <row r="66" spans="1:13" ht="14.25" customHeight="1">
+    <row r="66" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A66" s="79" t="s">
         <v>242</v>
       </c>
@@ -4943,7 +4944,7 @@
       </c>
       <c r="M66" s="34"/>
     </row>
-    <row r="67" spans="1:13" ht="14.25" customHeight="1">
+    <row r="67" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A67" s="79" t="s">
         <v>244</v>
       </c>
@@ -4983,7 +4984,7 @@
       </c>
       <c r="M67" s="34"/>
     </row>
-    <row r="68" spans="1:13" ht="14.25" customHeight="1">
+    <row r="68" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A68" s="79" t="s">
         <v>246</v>
       </c>
@@ -5023,7 +5024,7 @@
       </c>
       <c r="M68" s="34"/>
     </row>
-    <row r="69" spans="1:13" ht="14.25" customHeight="1">
+    <row r="69" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A69" s="79" t="s">
         <v>250</v>
       </c>
@@ -5063,7 +5064,7 @@
       </c>
       <c r="M69" s="34"/>
     </row>
-    <row r="70" spans="1:13" ht="14.25" customHeight="1">
+    <row r="70" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A70" s="79" t="s">
         <v>253</v>
       </c>
@@ -5103,7 +5104,7 @@
       </c>
       <c r="M70" s="34"/>
     </row>
-    <row r="71" spans="1:13" ht="14.25" customHeight="1">
+    <row r="71" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A71" s="79" t="s">
         <v>256</v>
       </c>
@@ -5143,7 +5144,7 @@
       </c>
       <c r="M71" s="34"/>
     </row>
-    <row r="72" spans="1:13" ht="14.25" customHeight="1">
+    <row r="72" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A72" s="79" t="s">
         <v>259</v>
       </c>
@@ -5183,7 +5184,7 @@
       </c>
       <c r="M72" s="34"/>
     </row>
-    <row r="73" spans="1:13" ht="14.25" customHeight="1">
+    <row r="73" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A73" s="87" t="s">
         <v>262</v>
       </c>
@@ -5223,7 +5224,7 @@
       </c>
       <c r="M73" s="34"/>
     </row>
-    <row r="74" spans="1:13" ht="14.25" customHeight="1">
+    <row r="74" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A74" s="79" t="s">
         <v>264</v>
       </c>
@@ -5263,7 +5264,7 @@
       </c>
       <c r="M74" s="34"/>
     </row>
-    <row r="75" spans="1:13" ht="14.25" customHeight="1">
+    <row r="75" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A75" s="79" t="s">
         <v>267</v>
       </c>
@@ -5304,7 +5305,7 @@
       </c>
       <c r="M75" s="34"/>
     </row>
-    <row r="76" spans="1:13" ht="14.25" customHeight="1">
+    <row r="76" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A76" s="79" t="s">
         <v>269</v>
       </c>
@@ -5344,7 +5345,7 @@
       </c>
       <c r="M76" s="34"/>
     </row>
-    <row r="77" spans="1:13" ht="14.25" customHeight="1">
+    <row r="77" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A77" s="79" t="s">
         <v>272</v>
       </c>
@@ -5384,7 +5385,7 @@
       </c>
       <c r="M77" s="34"/>
     </row>
-    <row r="78" spans="1:13" ht="14.25" customHeight="1">
+    <row r="78" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A78" s="79" t="s">
         <v>274</v>
       </c>
@@ -5424,7 +5425,7 @@
       </c>
       <c r="M78" s="34"/>
     </row>
-    <row r="79" spans="1:13" ht="14.25" customHeight="1">
+    <row r="79" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A79" s="87" t="s">
         <v>277</v>
       </c>
@@ -5463,7 +5464,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="14.25" customHeight="1">
+    <row r="80" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A80" s="79" t="s">
         <v>280</v>
       </c>
@@ -5500,7 +5501,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="14.25" customHeight="1">
+    <row r="81" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A81" s="79" t="s">
         <v>283</v>
       </c>
@@ -5835,7 +5836,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="14.25" customHeight="1">
+    <row r="90" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A90" s="139" t="s">
         <v>310</v>
       </c>
@@ -5868,7 +5869,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="14.25" customHeight="1">
+    <row r="91" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A91" s="139" t="s">
         <v>312</v>
       </c>
@@ -5901,7 +5902,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="14.25" customHeight="1">
+    <row r="92" spans="1:13" ht="14.25" hidden="1" customHeight="1">
       <c r="A92" s="145" t="s">
         <v>314</v>
       </c>
@@ -6076,7 +6077,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="14.25" customHeight="1">
+    <row r="97" spans="1:12" ht="14.25" hidden="1" customHeight="1">
       <c r="A97" s="120" t="s">
         <v>11</v>
       </c>
@@ -6181,7 +6182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="14.25" customHeight="1">
+    <row r="100" spans="1:12" ht="14.25" hidden="1" customHeight="1">
       <c r="A100" s="150" t="s">
         <v>26</v>
       </c>
@@ -6218,7 +6219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="14.25" customHeight="1">
+    <row r="101" spans="1:12" ht="14.25" hidden="1" customHeight="1">
       <c r="A101" s="150" t="s">
         <v>29</v>
       </c>
@@ -6255,7 +6256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="14.25" customHeight="1">
+    <row r="102" spans="1:12" ht="14.25" hidden="1" customHeight="1">
       <c r="A102" s="155" t="s">
         <v>31</v>
       </c>
@@ -6288,7 +6289,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="14.25">
+    <row r="103" spans="1:12" ht="14.25" hidden="1">
       <c r="A103" s="89" t="s">
         <v>361</v>
       </c>
@@ -6327,7 +6328,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="14.25">
+    <row r="104" spans="1:12" ht="14.25" hidden="1">
       <c r="A104" s="92" t="s">
         <v>364</v>
       </c>
@@ -6366,7 +6367,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="105" spans="1:12" s="93" customFormat="1" ht="14.25">
+    <row r="105" spans="1:12" s="93" customFormat="1" ht="14.25" hidden="1">
       <c r="A105" s="92" t="s">
         <v>371</v>
       </c>
@@ -6401,7 +6402,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="106" spans="1:12" s="93" customFormat="1" ht="14.25">
+    <row r="106" spans="1:12" s="93" customFormat="1" ht="14.25" hidden="1">
       <c r="A106" s="92" t="s">
         <v>375</v>
       </c>
@@ -15953,7 +15954,13 @@
       <c r="L970" s="66"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:L106"/>
+  <autoFilter ref="A4:L106">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Digikey"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="A1:L1"/>
@@ -16043,9 +16050,11 @@
     <hyperlink ref="L105" r:id="rId81"/>
     <hyperlink ref="L106" r:id="rId82"/>
     <hyperlink ref="L91" r:id="rId83"/>
+    <hyperlink ref="L17" r:id="rId84"/>
+    <hyperlink ref="L18" r:id="rId85"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId84"/>
+  <pageSetup orientation="portrait" r:id="rId86"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Absolute Encoder to a different model
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eddy/Documents/Development/Personal/open-source-rover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{711ADF74-5CED-174D-A631-869662F04C2A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3A65A5E0-8394-F64C-AB3B-35DFED3225DB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -808,9 +808,6 @@
     <t>E7</t>
   </si>
   <si>
-    <t>1/8 inch, 10 Bit Analog, Ball bearing</t>
-  </si>
-  <si>
     <t>Black Wire 30AWG</t>
   </si>
   <si>
@@ -1118,6 +1115,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>1/8 inch, 10 Bit Analog, Sleeve Bushing (N)</t>
   </si>
 </sst>
 </file>
@@ -1138,26 +1138,31 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1237,6 +1242,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1277,7 +1283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1336,19 +1342,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1387,7 +1380,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1469,16 +1462,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1494,7 +1487,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1515,13 +1508,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1669,10 +1662,10 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1696,36 +1689,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2038,45 +2034,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="109" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="121" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="123"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="122"/>
+    </row>
+    <row r="2" spans="1:27" s="111" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="124" t="s">
         <v>356</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-    </row>
-    <row r="2" spans="1:27" s="111" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="123" t="s">
-        <v>357</v>
-      </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
       <c r="G2" s="114"/>
       <c r="H2" s="114"/>
       <c r="I2" s="114"/>
-      <c r="J2" s="125" t="s">
-        <v>364</v>
-      </c>
-      <c r="K2" s="126">
+      <c r="J2" s="126" t="s">
+        <v>363</v>
+      </c>
+      <c r="K2" s="127">
         <f>SUM(K5:K150)</f>
-        <v>2519.5</v>
+        <v>2494.3000000000002</v>
       </c>
       <c r="L2" s="114"/>
     </row>
     <row r="3" spans="1:27" s="111" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="115" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B3" s="115"/>
       <c r="C3" s="115"/>
@@ -2114,7 +2110,7 @@
         <v>6</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>7</v>
@@ -2222,7 +2218,7 @@
         <v>37</v>
       </c>
       <c r="M6" s="10"/>
-      <c r="N6" s="118" t="s">
+      <c r="N6" s="119" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2263,7 +2259,7 @@
         <v>42</v>
       </c>
       <c r="M7" s="11"/>
-      <c r="N7" s="119"/>
+      <c r="N7" s="120"/>
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
@@ -2449,7 +2445,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J12" s="23">
         <v>9.25</v>
@@ -2620,7 +2616,7 @@
     </row>
     <row r="17" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B17" s="39">
         <v>25</v>
@@ -2638,7 +2634,7 @@
         <v>74</v>
       </c>
       <c r="G17" s="116" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H17" s="39" t="s">
         <v>12</v>
@@ -2652,13 +2648,13 @@
         <v>0.72</v>
       </c>
       <c r="L17" s="117" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B18" s="39">
         <v>25</v>
@@ -2676,7 +2672,7 @@
         <v>53</v>
       </c>
       <c r="G18" s="116" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H18" s="39" t="s">
         <v>12</v>
@@ -2690,7 +2686,7 @@
         <v>0.72</v>
       </c>
       <c r="L18" s="110" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M18" s="9"/>
     </row>
@@ -2766,7 +2762,7 @@
         <v>4.49</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M20" s="9"/>
     </row>
@@ -2796,7 +2792,7 @@
         <v>58</v>
       </c>
       <c r="I21" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J21" s="23">
         <v>25.27</v>
@@ -2836,7 +2832,7 @@
         <v>58</v>
       </c>
       <c r="I22" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J22" s="23">
         <v>12.9</v>
@@ -2876,7 +2872,7 @@
         <v>58</v>
       </c>
       <c r="I23" s="61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J23" s="23">
         <f>38.9+36.9</f>
@@ -2893,7 +2889,7 @@
     </row>
     <row r="24" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B24" s="39">
         <v>300</v>
@@ -2918,7 +2914,7 @@
         <v>93</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J24" s="23">
         <v>3.45</v>
@@ -2958,7 +2954,7 @@
         <v>93</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J25" s="23">
         <v>5.61</v>
@@ -3002,7 +2998,7 @@
         <v>93</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J26" s="23">
         <v>2.72</v>
@@ -3045,7 +3041,7 @@
         <v>93</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J27" s="23">
         <v>2.79</v>
@@ -3064,7 +3060,7 @@
     </row>
     <row r="28" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B28" s="39">
         <v>100</v>
@@ -3089,7 +3085,7 @@
         <v>93</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J28" s="23">
         <v>3.72</v>
@@ -3099,7 +3095,7 @@
         <v>3.72</v>
       </c>
       <c r="L28" s="27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M28" s="9"/>
       <c r="Y28" s="9"/>
@@ -3108,7 +3104,7 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B29" s="39">
         <v>100</v>
@@ -3132,7 +3128,7 @@
         <v>93</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J29" s="23">
         <v>3.72</v>
@@ -3142,7 +3138,7 @@
         <v>3.72</v>
       </c>
       <c r="L29" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M29" s="9"/>
       <c r="Y29" s="9"/>
@@ -3151,7 +3147,7 @@
     </row>
     <row r="30" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B30" s="41">
         <v>100</v>
@@ -3175,7 +3171,7 @@
         <v>93</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J30" s="23">
         <v>4.07</v>
@@ -3185,13 +3181,13 @@
         <v>4.07</v>
       </c>
       <c r="L30" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B31" s="41">
         <v>100</v>
@@ -3215,7 +3211,7 @@
         <v>93</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J31" s="23">
         <v>4.41</v>
@@ -3225,13 +3221,13 @@
         <v>4.41</v>
       </c>
       <c r="L31" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M31" s="9"/>
     </row>
     <row r="32" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B32" s="41">
         <v>50</v>
@@ -3255,7 +3251,7 @@
         <v>93</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J32" s="23">
         <v>5.42</v>
@@ -3265,13 +3261,13 @@
         <v>5.42</v>
       </c>
       <c r="L32" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M32" s="9"/>
     </row>
     <row r="33" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B33" s="39">
         <v>50</v>
@@ -3295,7 +3291,7 @@
         <v>93</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J33" s="23">
         <v>6.51</v>
@@ -3305,13 +3301,13 @@
         <v>6.51</v>
       </c>
       <c r="L33" s="27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M33" s="9"/>
     </row>
     <row r="34" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B34" s="39">
         <v>100</v>
@@ -3335,7 +3331,7 @@
         <v>93</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J34" s="23">
         <v>2.87</v>
@@ -3351,7 +3347,7 @@
     </row>
     <row r="35" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B35" s="41">
         <v>100</v>
@@ -3375,7 +3371,7 @@
         <v>93</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J35" s="23">
         <v>7.7</v>
@@ -3385,7 +3381,7 @@
         <v>7.7</v>
       </c>
       <c r="L35" s="26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -3409,13 +3405,13 @@
         <v>126</v>
       </c>
       <c r="G36" s="43" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H36" s="39" t="s">
         <v>58</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J36" s="23">
         <v>23.16</v>
@@ -3425,7 +3421,7 @@
         <v>23.16</v>
       </c>
       <c r="L36" s="110" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -3455,7 +3451,7 @@
         <v>58</v>
       </c>
       <c r="I37" s="61" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J37" s="23">
         <v>2.2599999999999998</v>
@@ -3495,7 +3491,7 @@
         <v>58</v>
       </c>
       <c r="I38" s="61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J38" s="23">
         <v>4.92</v>
@@ -3535,7 +3531,7 @@
         <v>93</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J39" s="23">
         <v>0.23</v>
@@ -3575,7 +3571,7 @@
         <v>93</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J40" s="23">
         <v>0.3</v>
@@ -3616,7 +3612,7 @@
         <v>93</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J41" s="23">
         <v>0.23</v>
@@ -3656,7 +3652,7 @@
         <v>93</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J42" s="23">
         <v>0.27</v>
@@ -3699,7 +3695,7 @@
         <v>93</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J43" s="23">
         <v>0.37</v>
@@ -3742,7 +3738,7 @@
         <v>93</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J44" s="23">
         <v>0.48</v>
@@ -3785,7 +3781,7 @@
         <v>93</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J45" s="23">
         <v>1.17</v>
@@ -3828,7 +3824,7 @@
         <v>93</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J46" s="23">
         <v>1.4</v>
@@ -3868,7 +3864,7 @@
         <v>93</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J47" s="23">
         <v>2.4700000000000002</v>
@@ -3992,7 +3988,7 @@
         <v>209.70000000000002</v>
       </c>
       <c r="L50" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M50" s="9"/>
     </row>
@@ -4060,7 +4056,7 @@
         <v>58</v>
       </c>
       <c r="I52" s="61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J52" s="23">
         <v>2.99</v>
@@ -4100,7 +4096,7 @@
         <v>58</v>
       </c>
       <c r="I53" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J53" s="23">
         <v>5.99</v>
@@ -4140,7 +4136,7 @@
         <v>58</v>
       </c>
       <c r="I54" s="61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J54" s="23">
         <v>6.99</v>
@@ -4180,7 +4176,7 @@
         <v>58</v>
       </c>
       <c r="I55" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J55" s="23">
         <v>5.99</v>
@@ -4220,7 +4216,7 @@
         <v>58</v>
       </c>
       <c r="I56" s="61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J56" s="23">
         <v>5.99</v>
@@ -4260,7 +4256,7 @@
         <v>58</v>
       </c>
       <c r="I57" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J57" s="23">
         <v>5.99</v>
@@ -4300,7 +4296,7 @@
         <v>58</v>
       </c>
       <c r="I58" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J58" s="23">
         <v>1.49</v>
@@ -4340,12 +4336,12 @@
         <v>58</v>
       </c>
       <c r="I59" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J59" s="23">
         <v>5.99</v>
       </c>
-      <c r="K59" s="124">
+      <c r="K59" s="118">
         <f t="shared" si="1"/>
         <v>47.92</v>
       </c>
@@ -4380,7 +4376,7 @@
         <v>58</v>
       </c>
       <c r="I60" s="25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J60" s="23">
         <v>2.09</v>
@@ -4420,7 +4416,7 @@
         <v>58</v>
       </c>
       <c r="I61" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J61" s="23">
         <v>1.49</v>
@@ -4460,7 +4456,7 @@
         <v>58</v>
       </c>
       <c r="I62" s="61" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J62" s="23">
         <v>3.99</v>
@@ -4500,7 +4496,7 @@
         <v>58</v>
       </c>
       <c r="I63" s="61" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J63" s="23">
         <v>5.99</v>
@@ -4540,7 +4536,7 @@
         <v>58</v>
       </c>
       <c r="I64" s="61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J64" s="23">
         <v>2.39</v>
@@ -4580,7 +4576,7 @@
         <v>58</v>
       </c>
       <c r="I65" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J65" s="23">
         <v>4.99</v>
@@ -4620,7 +4616,7 @@
         <v>58</v>
       </c>
       <c r="I66" s="61" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J66" s="23">
         <v>9.99</v>
@@ -4660,7 +4656,7 @@
         <v>58</v>
       </c>
       <c r="I67" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J67" s="23">
         <v>5.99</v>
@@ -4700,7 +4696,7 @@
         <v>58</v>
       </c>
       <c r="I68" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J68" s="23">
         <v>3.69</v>
@@ -4740,7 +4736,7 @@
         <v>58</v>
       </c>
       <c r="I69" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J69" s="23">
         <v>7.99</v>
@@ -4780,7 +4776,7 @@
         <v>58</v>
       </c>
       <c r="I70" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J70" s="23">
         <v>4.49</v>
@@ -4820,7 +4816,7 @@
         <v>58</v>
       </c>
       <c r="I71" s="61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J71" s="23">
         <v>16.989999999999998</v>
@@ -4860,7 +4856,7 @@
         <v>58</v>
       </c>
       <c r="I72" s="61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J72" s="23">
         <v>13.99</v>
@@ -4900,7 +4896,7 @@
         <v>58</v>
       </c>
       <c r="I73" s="73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J73" s="23">
         <v>4.99</v>
@@ -4940,7 +4936,7 @@
         <v>58</v>
       </c>
       <c r="I74" s="61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J74" s="23">
         <v>7.99</v>
@@ -4981,7 +4977,7 @@
         <v>58</v>
       </c>
       <c r="I75" s="61" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J75" s="23">
         <v>3.99</v>
@@ -5021,7 +5017,7 @@
         <v>58</v>
       </c>
       <c r="I76" s="61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J76" s="23">
         <v>2.79</v>
@@ -5061,7 +5057,7 @@
         <v>58</v>
       </c>
       <c r="I77" s="61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J77" s="23">
         <v>1.29</v>
@@ -5101,7 +5097,7 @@
         <v>58</v>
       </c>
       <c r="I78" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J78" s="23">
         <v>3.99</v>
@@ -5141,7 +5137,7 @@
         <v>93</v>
       </c>
       <c r="I79" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J79" s="23">
         <v>1.79</v>
@@ -5174,7 +5170,7 @@
         <v>258</v>
       </c>
       <c r="G80" s="43" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H80" s="60" t="s">
         <v>12</v>
@@ -5211,18 +5207,18 @@
         <v>260</v>
       </c>
       <c r="G81" s="43" t="s">
-        <v>261</v>
+        <v>364</v>
       </c>
       <c r="H81" s="60" t="s">
         <v>12</v>
       </c>
       <c r="I81" s="61"/>
       <c r="J81" s="75">
-        <v>61.3</v>
+        <v>55</v>
       </c>
       <c r="K81" s="23">
         <f t="shared" si="2"/>
-        <v>245.2</v>
+        <v>220</v>
       </c>
       <c r="L81" s="28" t="s">
         <v>259</v>
@@ -5230,7 +5226,7 @@
     </row>
     <row r="82" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B82" s="41">
         <v>1</v>
@@ -5248,7 +5244,7 @@
         <v>19</v>
       </c>
       <c r="G82" s="47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H82" s="41" t="s">
         <v>12</v>
@@ -5262,13 +5258,13 @@
         <v>6.32</v>
       </c>
       <c r="L82" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M82" s="15"/>
     </row>
     <row r="83" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B83" s="41">
         <v>1</v>
@@ -5286,7 +5282,7 @@
         <v>19</v>
       </c>
       <c r="G83" s="43" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H83" s="41" t="s">
         <v>12</v>
@@ -5300,12 +5296,12 @@
         <v>6.14</v>
       </c>
       <c r="L83" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B84" s="41">
         <v>1</v>
@@ -5323,7 +5319,7 @@
         <v>19</v>
       </c>
       <c r="G84" s="47" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H84" s="41" t="s">
         <v>12</v>
@@ -5337,12 +5333,12 @@
         <v>4.95</v>
       </c>
       <c r="L84" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B85" s="41">
         <v>1</v>
@@ -5360,7 +5356,7 @@
         <v>19</v>
       </c>
       <c r="G85" s="47" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H85" s="41" t="s">
         <v>12</v>
@@ -5374,12 +5370,12 @@
         <v>4.95</v>
       </c>
       <c r="L85" s="41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B86" s="41">
         <v>1</v>
@@ -5397,7 +5393,7 @@
         <v>19</v>
       </c>
       <c r="G86" s="47" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H86" s="41" t="s">
         <v>12</v>
@@ -5411,13 +5407,13 @@
         <v>4.95</v>
       </c>
       <c r="L86" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M86" s="15"/>
     </row>
     <row r="87" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B87" s="41">
         <v>1</v>
@@ -5435,7 +5431,7 @@
         <v>19</v>
       </c>
       <c r="G87" s="47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H87" s="41" t="s">
         <v>12</v>
@@ -5449,12 +5445,12 @@
         <v>4.95</v>
       </c>
       <c r="L87" s="41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="76" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B88" s="41">
         <v>10</v>
@@ -5470,7 +5466,7 @@
       </c>
       <c r="F88" s="41"/>
       <c r="G88" s="106" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H88" s="41" t="s">
         <v>12</v>
@@ -5484,12 +5480,12 @@
         <v>3.67</v>
       </c>
       <c r="L88" s="77" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="78" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B89" s="72">
         <v>10</v>
@@ -5505,7 +5501,7 @@
       </c>
       <c r="F89" s="72"/>
       <c r="G89" s="107" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H89" s="72" t="s">
         <v>12</v>
@@ -5519,12 +5515,12 @@
         <v>0.4</v>
       </c>
       <c r="L89" s="80" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="81" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B90" s="82">
         <v>0</v>
@@ -5552,12 +5548,12 @@
         <v>0</v>
       </c>
       <c r="L90" s="82" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="81" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B91" s="82">
         <v>0</v>
@@ -5585,12 +5581,12 @@
         <v>0</v>
       </c>
       <c r="L91" s="86" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="87" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B92" s="72">
         <v>1</v>
@@ -5606,7 +5602,7 @@
       </c>
       <c r="F92" s="72"/>
       <c r="G92" s="88" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H92" s="72" t="s">
         <v>12</v>
@@ -5620,12 +5616,12 @@
         <v>7.99</v>
       </c>
       <c r="L92" s="89" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="87" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B93" s="72">
         <v>1</v>
@@ -5641,7 +5637,7 @@
       </c>
       <c r="F93" s="72"/>
       <c r="G93" s="88" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H93" s="72" t="s">
         <v>12</v>
@@ -5655,12 +5651,12 @@
         <v>15.59</v>
       </c>
       <c r="L93" s="89" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="87" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B94" s="72">
         <v>1</v>
@@ -5676,7 +5672,7 @@
       </c>
       <c r="F94" s="72"/>
       <c r="G94" s="88" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H94" s="72" t="s">
         <v>12</v>
@@ -5690,12 +5686,12 @@
         <v>12.56</v>
       </c>
       <c r="L94" s="90" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="87" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B95" s="72">
         <v>1</v>
@@ -5711,7 +5707,7 @@
       </c>
       <c r="F95" s="72"/>
       <c r="G95" s="88" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H95" s="72" t="s">
         <v>12</v>
@@ -5725,12 +5721,12 @@
         <v>15.59</v>
       </c>
       <c r="L95" s="89" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="87" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B96" s="72">
         <v>1</v>
@@ -5746,7 +5742,7 @@
       </c>
       <c r="F96" s="72"/>
       <c r="G96" s="88" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H96" s="72" t="s">
         <v>12</v>
@@ -5760,7 +5756,7 @@
         <v>15.59</v>
       </c>
       <c r="L96" s="89" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5781,7 +5777,7 @@
       </c>
       <c r="F97" s="63"/>
       <c r="G97" s="68" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H97" s="63" t="s">
         <v>12</v>
@@ -5795,7 +5791,7 @@
         <v>19.75</v>
       </c>
       <c r="L97" s="69" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5977,7 +5973,7 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B103" s="42">
         <v>25</v>
@@ -5992,16 +5988,16 @@
         <v>90</v>
       </c>
       <c r="F103" s="42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G103" s="108" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H103" s="49" t="s">
         <v>93</v>
       </c>
       <c r="I103" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J103" s="33">
         <v>3.78</v>
@@ -6011,12 +6007,12 @@
         <v>3.78</v>
       </c>
       <c r="L103" s="103" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B104" s="42">
         <v>4</v>
@@ -6031,16 +6027,16 @@
         <v>90</v>
       </c>
       <c r="F104" s="42" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G104" s="50" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H104" s="51" t="s">
         <v>93</v>
       </c>
       <c r="I104" s="32" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J104" s="33">
         <v>0.96</v>
@@ -6050,12 +6046,12 @@
         <v>3.84</v>
       </c>
       <c r="L104" s="103" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="34" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B105" s="42">
         <v>1</v>
@@ -6067,10 +6063,10 @@
         <v>1</v>
       </c>
       <c r="E105" s="42" t="s">
+        <v>343</v>
+      </c>
+      <c r="F105" s="42" t="s">
         <v>344</v>
-      </c>
-      <c r="F105" s="42" t="s">
-        <v>345</v>
       </c>
       <c r="G105" s="104"/>
       <c r="H105" s="51" t="s">
@@ -6085,12 +6081,12 @@
         <v>11.75</v>
       </c>
       <c r="L105" s="103" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="106" spans="1:12" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B106" s="42">
         <v>1</v>
@@ -6102,7 +6098,7 @@
         <v>1</v>
       </c>
       <c r="E106" s="42" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F106" s="42" t="s">
         <v>170</v>
@@ -6120,7 +6116,7 @@
         <v>15.25</v>
       </c>
       <c r="L106" s="103" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6151,7 +6147,7 @@
       <c r="C109" s="17"/>
       <c r="D109" s="18"/>
       <c r="E109" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F109" s="20">
         <v>10</v>
@@ -6168,7 +6164,7 @@
       <c r="C110" s="17"/>
       <c r="D110" s="18"/>
       <c r="E110" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F110" s="20">
         <v>10</v>

</xml_diff>

<commit_message>
Fixed Absolute Encoder price
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eddy/Documents/Development/Personal/open-source-rover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3A65A5E0-8394-F64C-AB3B-35DFED3225DB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C562BB8E-8300-8744-888A-186717FFB17D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1702,6 +1702,10 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1715,16 +1719,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -2034,39 +2034,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="109" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="123" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="122"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="124"/>
     </row>
     <row r="2" spans="1:27" s="111" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="127" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="124"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
       <c r="G2" s="114"/>
       <c r="H2" s="114"/>
       <c r="I2" s="114"/>
-      <c r="J2" s="126" t="s">
+      <c r="J2" s="119" t="s">
         <v>363</v>
       </c>
-      <c r="K2" s="127">
+      <c r="K2" s="120">
         <f>SUM(K5:K150)</f>
-        <v>2494.3000000000002</v>
+        <v>2496.3000000000002</v>
       </c>
       <c r="L2" s="114"/>
     </row>
@@ -2218,7 +2218,7 @@
         <v>37</v>
       </c>
       <c r="M6" s="10"/>
-      <c r="N6" s="119" t="s">
+      <c r="N6" s="121" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2259,7 +2259,7 @@
         <v>42</v>
       </c>
       <c r="M7" s="11"/>
-      <c r="N7" s="120"/>
+      <c r="N7" s="122"/>
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
@@ -5214,11 +5214,11 @@
       </c>
       <c r="I81" s="61"/>
       <c r="J81" s="75">
-        <v>55</v>
+        <v>55.5</v>
       </c>
       <c r="K81" s="23">
         <f t="shared" si="2"/>
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="L81" s="28" t="s">
         <v>259</v>

</xml_diff>

<commit_message>
Fixed total price formula
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eddy/Documents/Development/Personal/open-source-rover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8DC9723C-173E-D945-AF45-E5216D3C2181}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EF0CBBAA-F93B-5E4D-A359-A4DD09EA7AB9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1130,7 +1130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1206,14 +1206,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1375,9 +1367,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1578,9 +1570,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1623,10 +1612,10 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1655,7 +1644,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1683,28 +1672,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1716,11 +1704,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -2029,7 +2015,7 @@
     <col min="15" max="27" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="106" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="105" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="120" t="s">
         <v>355</v>
       </c>
@@ -2045,7 +2031,7 @@
       <c r="K1" s="123"/>
       <c r="L1" s="121"/>
     </row>
-    <row r="2" spans="1:27" s="108" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="107" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="124" t="s">
         <v>356</v>
       </c>
@@ -2054,31 +2040,31 @@
       <c r="D2" s="124"/>
       <c r="E2" s="124"/>
       <c r="F2" s="124"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="116" t="s">
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="114" t="s">
         <v>362</v>
       </c>
-      <c r="K2" s="117">
+      <c r="K2" s="115">
         <f>SUM(K5:K150)</f>
-        <v>2297.8784000000001</v>
-      </c>
-      <c r="L2" s="111"/>
-    </row>
-    <row r="3" spans="1:27" s="108" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="112" t="s">
+        <v>2466.1200000000003</v>
+      </c>
+      <c r="L2" s="110"/>
+    </row>
+    <row r="3" spans="1:27" s="107" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="111" t="s">
         <v>357</v>
       </c>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="109"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="108"/>
     </row>
     <row r="4" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -2163,7 +2149,7 @@
         <v>1.5</v>
       </c>
       <c r="K5" s="56">
-        <f t="shared" ref="K5:K13" si="0">B5/D5*J5</f>
+        <f>B5*J5</f>
         <v>3</v>
       </c>
       <c r="L5" s="57" t="s">
@@ -2206,8 +2192,8 @@
       <c r="J6" s="22">
         <v>34.99</v>
       </c>
-      <c r="K6" s="22">
-        <f t="shared" si="0"/>
+      <c r="K6" s="56">
+        <f t="shared" ref="K6:K69" si="0">B6*J6</f>
         <v>34.99</v>
       </c>
       <c r="L6" s="27" t="s">
@@ -2247,7 +2233,7 @@
       <c r="J7" s="64">
         <v>25</v>
       </c>
-      <c r="K7" s="64">
+      <c r="K7" s="56">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -2256,9 +2242,9 @@
       </c>
       <c r="M7" s="11"/>
       <c r="N7" s="119"/>
-      <c r="Y7" s="126"/>
-      <c r="Z7" s="126"/>
-      <c r="AA7" s="126"/>
+      <c r="Y7" s="117"/>
+      <c r="Z7" s="117"/>
+      <c r="AA7" s="117"/>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
@@ -2289,7 +2275,7 @@
       <c r="J8" s="22">
         <v>13.24</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="56">
         <f t="shared" si="0"/>
         <v>13.24</v>
       </c>
@@ -2297,9 +2283,9 @@
         <v>43</v>
       </c>
       <c r="M8" s="9"/>
-      <c r="Y8" s="126"/>
-      <c r="Z8" s="126"/>
-      <c r="AA8" s="126"/>
+      <c r="Y8" s="117"/>
+      <c r="Z8" s="117"/>
+      <c r="AA8" s="117"/>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
@@ -2330,7 +2316,7 @@
       <c r="J9" s="22">
         <v>9.98</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="56">
         <f t="shared" si="0"/>
         <v>9.98</v>
       </c>
@@ -2338,9 +2324,9 @@
         <v>48</v>
       </c>
       <c r="M9" s="9"/>
-      <c r="Y9" s="126"/>
-      <c r="Z9" s="126"/>
-      <c r="AA9" s="126"/>
+      <c r="Y9" s="117"/>
+      <c r="Z9" s="117"/>
+      <c r="AA9" s="117"/>
     </row>
     <row r="10" spans="1:27" s="36" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="60" t="s">
@@ -2371,7 +2357,7 @@
       <c r="J10" s="64">
         <v>6.79</v>
       </c>
-      <c r="K10" s="64">
+      <c r="K10" s="56">
         <f t="shared" si="0"/>
         <v>6.79</v>
       </c>
@@ -2379,9 +2365,9 @@
         <v>51</v>
       </c>
       <c r="M10" s="35"/>
-      <c r="Y10" s="126"/>
-      <c r="Z10" s="126"/>
-      <c r="AA10" s="126"/>
+      <c r="Y10" s="117"/>
+      <c r="Z10" s="117"/>
+      <c r="AA10" s="117"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
@@ -2412,7 +2398,7 @@
       <c r="J11" s="22">
         <v>5.57</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="56">
         <f t="shared" si="0"/>
         <v>5.57</v>
       </c>
@@ -2420,9 +2406,9 @@
         <v>54</v>
       </c>
       <c r="M11" s="9"/>
-      <c r="Y11" s="126"/>
-      <c r="Z11" s="126"/>
-      <c r="AA11" s="126"/>
+      <c r="Y11" s="117"/>
+      <c r="Z11" s="117"/>
+      <c r="AA11" s="117"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
@@ -2455,17 +2441,17 @@
       <c r="J12" s="22">
         <v>9.25</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="56">
         <f t="shared" si="0"/>
-        <v>9.25</v>
+        <v>18.5</v>
       </c>
       <c r="L12" s="27" t="s">
         <v>59</v>
       </c>
       <c r="M12" s="12"/>
-      <c r="Y12" s="126"/>
-      <c r="Z12" s="126"/>
-      <c r="AA12" s="126"/>
+      <c r="Y12" s="117"/>
+      <c r="Z12" s="117"/>
+      <c r="AA12" s="117"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
@@ -2496,7 +2482,7 @@
       <c r="J13" s="22">
         <v>6.49</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="56">
         <f t="shared" si="0"/>
         <v>6.49</v>
       </c>
@@ -2504,9 +2490,9 @@
         <v>63</v>
       </c>
       <c r="M13" s="9"/>
-      <c r="Y13" s="126"/>
-      <c r="Z13" s="126"/>
-      <c r="AA13" s="126"/>
+      <c r="Y13" s="117"/>
+      <c r="Z13" s="117"/>
+      <c r="AA13" s="117"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
@@ -2537,8 +2523,8 @@
       <c r="J14" s="22">
         <v>5.42</v>
       </c>
-      <c r="K14" s="22">
-        <f>J14</f>
+      <c r="K14" s="56">
+        <f t="shared" si="0"/>
         <v>5.42</v>
       </c>
       <c r="L14" s="27" t="s">
@@ -2546,7 +2532,7 @@
       </c>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:27" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>67</v>
       </c>
@@ -2575,8 +2561,8 @@
       <c r="J15" s="22">
         <v>86.95</v>
       </c>
-      <c r="K15" s="22">
-        <f t="shared" ref="K15:K59" si="1">B15/D15*J15</f>
+      <c r="K15" s="56">
+        <f t="shared" si="0"/>
         <v>86.95</v>
       </c>
       <c r="L15" s="27" t="s">
@@ -2613,8 +2599,8 @@
       <c r="J16" s="22">
         <v>41.95</v>
       </c>
-      <c r="K16" s="22">
-        <f t="shared" si="1"/>
+      <c r="K16" s="56">
+        <f t="shared" si="0"/>
         <v>41.95</v>
       </c>
       <c r="L16" s="27" t="s">
@@ -2641,7 +2627,7 @@
       <c r="F17" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="113" t="s">
+      <c r="G17" s="112" t="s">
         <v>358</v>
       </c>
       <c r="H17" s="37" t="s">
@@ -2651,11 +2637,11 @@
       <c r="J17" s="22">
         <v>0.04</v>
       </c>
-      <c r="K17" s="22">
-        <f t="shared" si="1"/>
+      <c r="K17" s="56">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="L17" s="114" t="s">
+      <c r="L17" s="113" t="s">
         <v>359</v>
       </c>
       <c r="M17" s="9"/>
@@ -2679,7 +2665,7 @@
       <c r="F18" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="113" t="s">
+      <c r="G18" s="112" t="s">
         <v>361</v>
       </c>
       <c r="H18" s="37" t="s">
@@ -2689,11 +2675,11 @@
       <c r="J18" s="22">
         <v>0.04</v>
       </c>
-      <c r="K18" s="22">
-        <f t="shared" si="1"/>
+      <c r="K18" s="56">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="L18" s="107" t="s">
+      <c r="L18" s="106" t="s">
         <v>360</v>
       </c>
       <c r="M18" s="9"/>
@@ -2727,8 +2713,8 @@
       <c r="J19" s="22">
         <v>24.95</v>
       </c>
-      <c r="K19" s="22">
-        <f t="shared" si="1"/>
+      <c r="K19" s="56">
+        <f t="shared" si="0"/>
         <v>24.95</v>
       </c>
       <c r="L19" s="27" t="s">
@@ -2765,8 +2751,8 @@
       <c r="J20" s="22">
         <v>4.49</v>
       </c>
-      <c r="K20" s="22">
-        <f t="shared" si="1"/>
+      <c r="K20" s="56">
+        <f t="shared" si="0"/>
         <v>4.49</v>
       </c>
       <c r="L20" s="29" t="s">
@@ -2805,9 +2791,9 @@
       <c r="J21" s="22">
         <v>25.27</v>
       </c>
-      <c r="K21" s="22">
-        <f t="shared" si="1"/>
-        <v>37.905000000000001</v>
+      <c r="K21" s="56">
+        <f t="shared" si="0"/>
+        <v>75.81</v>
       </c>
       <c r="L21" s="27" t="s">
         <v>83</v>
@@ -2845,8 +2831,8 @@
       <c r="J22" s="22">
         <v>12.9</v>
       </c>
-      <c r="K22" s="22">
-        <f t="shared" si="1"/>
+      <c r="K22" s="56">
+        <f t="shared" si="0"/>
         <v>51.6</v>
       </c>
       <c r="L22" s="27" t="s">
@@ -2886,8 +2872,8 @@
         <f>38.9+36.9</f>
         <v>75.8</v>
       </c>
-      <c r="K23" s="22">
-        <f t="shared" si="1"/>
+      <c r="K23" s="56">
+        <f t="shared" si="0"/>
         <v>75.8</v>
       </c>
       <c r="L23" s="27" t="s">
@@ -2927,9 +2913,9 @@
       <c r="J24" s="22">
         <v>3.45</v>
       </c>
-      <c r="K24" s="22">
-        <f t="shared" si="1"/>
-        <v>6.9000000000000006E-2</v>
+      <c r="K24" s="56">
+        <f t="shared" si="0"/>
+        <v>6.9</v>
       </c>
       <c r="L24" s="23" t="s">
         <v>94</v>
@@ -2967,9 +2953,9 @@
       <c r="J25" s="22">
         <v>5.61</v>
       </c>
-      <c r="K25" s="22">
-        <f t="shared" si="1"/>
-        <v>0.22440000000000002</v>
+      <c r="K25" s="56">
+        <f t="shared" si="0"/>
+        <v>5.61</v>
       </c>
       <c r="L25" s="25" t="str">
         <f>HYPERLINK("https://www.mcmaster.com/#91292A015","https://www.mcmaster.com/#91292A015")</f>
@@ -3011,9 +2997,9 @@
       <c r="J26" s="22">
         <v>2.72</v>
       </c>
-      <c r="K26" s="22">
-        <f t="shared" si="1"/>
-        <v>2.7200000000000002E-2</v>
+      <c r="K26" s="56">
+        <f t="shared" si="0"/>
+        <v>2.72</v>
       </c>
       <c r="L26" s="26" t="s">
         <v>101</v>
@@ -3054,9 +3040,9 @@
       <c r="J27" s="22">
         <v>2.79</v>
       </c>
-      <c r="K27" s="22">
-        <f t="shared" si="1"/>
-        <v>2.7900000000000001E-2</v>
+      <c r="K27" s="56">
+        <f t="shared" si="0"/>
+        <v>2.79</v>
       </c>
       <c r="L27" s="25" t="s">
         <v>105</v>
@@ -3098,9 +3084,9 @@
       <c r="J28" s="22">
         <v>3.72</v>
       </c>
-      <c r="K28" s="22">
-        <f t="shared" si="1"/>
-        <v>3.7200000000000004E-2</v>
+      <c r="K28" s="56">
+        <f t="shared" si="0"/>
+        <v>3.72</v>
       </c>
       <c r="L28" s="26" t="s">
         <v>324</v>
@@ -3141,9 +3127,9 @@
       <c r="J29" s="22">
         <v>3.72</v>
       </c>
-      <c r="K29" s="22">
-        <f t="shared" si="1"/>
-        <v>3.7200000000000004E-2</v>
+      <c r="K29" s="56">
+        <f t="shared" si="0"/>
+        <v>3.72</v>
       </c>
       <c r="L29" s="26" t="s">
         <v>321</v>
@@ -3184,9 +3170,9 @@
       <c r="J30" s="22">
         <v>4.07</v>
       </c>
-      <c r="K30" s="22">
-        <f t="shared" si="1"/>
-        <v>4.0700000000000007E-2</v>
+      <c r="K30" s="56">
+        <f t="shared" si="0"/>
+        <v>4.07</v>
       </c>
       <c r="L30" s="25" t="s">
         <v>325</v>
@@ -3224,9 +3210,9 @@
       <c r="J31" s="22">
         <v>4.41</v>
       </c>
-      <c r="K31" s="22">
-        <f t="shared" si="1"/>
-        <v>4.41E-2</v>
+      <c r="K31" s="56">
+        <f t="shared" si="0"/>
+        <v>4.41</v>
       </c>
       <c r="L31" s="25" t="s">
         <v>320</v>
@@ -3264,9 +3250,9 @@
       <c r="J32" s="22">
         <v>5.42</v>
       </c>
-      <c r="K32" s="22">
-        <f t="shared" si="1"/>
-        <v>0.1084</v>
+      <c r="K32" s="56">
+        <f t="shared" si="0"/>
+        <v>5.42</v>
       </c>
       <c r="L32" s="25" t="s">
         <v>328</v>
@@ -3304,9 +3290,9 @@
       <c r="J33" s="22">
         <v>6.51</v>
       </c>
-      <c r="K33" s="22">
-        <f t="shared" si="1"/>
-        <v>0.13020000000000001</v>
+      <c r="K33" s="56">
+        <f t="shared" si="0"/>
+        <v>6.51</v>
       </c>
       <c r="L33" s="26" t="s">
         <v>330</v>
@@ -3344,9 +3330,9 @@
       <c r="J34" s="22">
         <v>2.87</v>
       </c>
-      <c r="K34" s="22">
-        <f t="shared" si="1"/>
-        <v>2.8700000000000003E-2</v>
+      <c r="K34" s="56">
+        <f t="shared" si="0"/>
+        <v>2.87</v>
       </c>
       <c r="L34" s="26" t="s">
         <v>122</v>
@@ -3384,9 +3370,9 @@
       <c r="J35" s="22">
         <v>7.7</v>
       </c>
-      <c r="K35" s="22">
-        <f t="shared" si="1"/>
-        <v>7.6999999999999999E-2</v>
+      <c r="K35" s="56">
+        <f t="shared" si="0"/>
+        <v>7.7</v>
       </c>
       <c r="L35" s="25" t="s">
         <v>336</v>
@@ -3424,11 +3410,11 @@
       <c r="J36" s="22">
         <v>23.16</v>
       </c>
-      <c r="K36" s="22">
-        <f t="shared" si="1"/>
+      <c r="K36" s="56">
+        <f t="shared" si="0"/>
         <v>23.16</v>
       </c>
-      <c r="L36" s="107" t="s">
+      <c r="L36" s="106" t="s">
         <v>354</v>
       </c>
       <c r="M36" s="9"/>
@@ -3464,8 +3450,8 @@
       <c r="J37" s="22">
         <v>2.2599999999999998</v>
       </c>
-      <c r="K37" s="22">
-        <f t="shared" si="1"/>
+      <c r="K37" s="56">
+        <f t="shared" si="0"/>
         <v>24.86</v>
       </c>
       <c r="L37" s="27" t="s">
@@ -3504,8 +3490,8 @@
       <c r="J38" s="22">
         <v>4.92</v>
       </c>
-      <c r="K38" s="22">
-        <f t="shared" si="1"/>
+      <c r="K38" s="56">
+        <f t="shared" si="0"/>
         <v>4.92</v>
       </c>
       <c r="L38" s="27" t="s">
@@ -3544,8 +3530,8 @@
       <c r="J39" s="22">
         <v>0.23</v>
       </c>
-      <c r="K39" s="22">
-        <f t="shared" si="1"/>
+      <c r="K39" s="56">
+        <f t="shared" si="0"/>
         <v>15.64</v>
       </c>
       <c r="L39" s="25" t="s">
@@ -3584,8 +3570,8 @@
       <c r="J40" s="22">
         <v>0.3</v>
       </c>
-      <c r="K40" s="22">
-        <f t="shared" si="1"/>
+      <c r="K40" s="56">
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="L40" s="27" t="str">
@@ -3625,8 +3611,8 @@
       <c r="J41" s="22">
         <v>0.23</v>
       </c>
-      <c r="K41" s="22">
-        <f t="shared" si="1"/>
+      <c r="K41" s="56">
+        <f t="shared" si="0"/>
         <v>2.3000000000000003</v>
       </c>
       <c r="L41" s="25" t="s">
@@ -3665,8 +3651,8 @@
       <c r="J42" s="22">
         <v>0.27</v>
       </c>
-      <c r="K42" s="22">
-        <f t="shared" si="1"/>
+      <c r="K42" s="56">
+        <f t="shared" si="0"/>
         <v>4.0500000000000007</v>
       </c>
       <c r="L42" s="25" t="s">
@@ -3708,8 +3694,8 @@
       <c r="J43" s="22">
         <v>0.37</v>
       </c>
-      <c r="K43" s="22">
-        <f t="shared" si="1"/>
+      <c r="K43" s="56">
+        <f t="shared" si="0"/>
         <v>3.7</v>
       </c>
       <c r="L43" s="26" t="s">
@@ -3751,8 +3737,8 @@
       <c r="J44" s="22">
         <v>0.48</v>
       </c>
-      <c r="K44" s="22">
-        <f t="shared" si="1"/>
+      <c r="K44" s="56">
+        <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
       <c r="L44" s="27" t="s">
@@ -3794,9 +3780,9 @@
       <c r="J45" s="22">
         <v>1.17</v>
       </c>
-      <c r="K45" s="22">
-        <f t="shared" si="1"/>
-        <v>1.17E-2</v>
+      <c r="K45" s="56">
+        <f t="shared" si="0"/>
+        <v>1.17</v>
       </c>
       <c r="L45" s="26" t="s">
         <v>161</v>
@@ -3837,9 +3823,9 @@
       <c r="J46" s="22">
         <v>1.4</v>
       </c>
-      <c r="K46" s="22">
-        <f t="shared" si="1"/>
-        <v>1.3999999999999999E-2</v>
+      <c r="K46" s="56">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
       </c>
       <c r="L46" s="29" t="s">
         <v>165</v>
@@ -3877,9 +3863,9 @@
       <c r="J47" s="22">
         <v>2.4700000000000002</v>
       </c>
-      <c r="K47" s="22">
-        <f t="shared" si="1"/>
-        <v>1.482</v>
+      <c r="K47" s="56">
+        <f t="shared" si="0"/>
+        <v>7.41</v>
       </c>
       <c r="L47" s="26" t="s">
         <v>169</v>
@@ -3915,8 +3901,8 @@
       <c r="J48" s="22">
         <v>69.95</v>
       </c>
-      <c r="K48" s="22">
-        <f t="shared" si="1"/>
+      <c r="K48" s="56">
+        <f t="shared" si="0"/>
         <v>349.75</v>
       </c>
       <c r="L48" s="27" t="s">
@@ -3953,8 +3939,8 @@
       <c r="J49" s="22">
         <v>14.95</v>
       </c>
-      <c r="K49" s="22">
-        <f t="shared" si="1"/>
+      <c r="K49" s="56">
+        <f t="shared" si="0"/>
         <v>14.95</v>
       </c>
       <c r="L49" s="27" t="s">
@@ -3991,11 +3977,11 @@
       <c r="J50" s="22">
         <v>34.950000000000003</v>
       </c>
-      <c r="K50" s="22">
-        <f t="shared" si="1"/>
+      <c r="K50" s="56">
+        <f t="shared" si="0"/>
         <v>209.70000000000002</v>
       </c>
-      <c r="L50" s="107" t="s">
+      <c r="L50" s="106" t="s">
         <v>364</v>
       </c>
       <c r="M50" s="9"/>
@@ -4029,8 +4015,8 @@
       <c r="J51" s="22">
         <v>19.95</v>
       </c>
-      <c r="K51" s="22">
-        <f t="shared" si="1"/>
+      <c r="K51" s="56">
+        <f t="shared" si="0"/>
         <v>79.8</v>
       </c>
       <c r="L51" s="27" t="s">
@@ -4069,8 +4055,8 @@
       <c r="J52" s="22">
         <v>2.99</v>
       </c>
-      <c r="K52" s="22">
-        <f t="shared" si="1"/>
+      <c r="K52" s="56">
+        <f t="shared" si="0"/>
         <v>17.940000000000001</v>
       </c>
       <c r="L52" s="27" t="s">
@@ -4109,8 +4095,8 @@
       <c r="J53" s="22">
         <v>5.99</v>
       </c>
-      <c r="K53" s="22">
-        <f t="shared" si="1"/>
+      <c r="K53" s="56">
+        <f t="shared" si="0"/>
         <v>47.92</v>
       </c>
       <c r="L53" s="27" t="s">
@@ -4149,8 +4135,8 @@
       <c r="J54" s="22">
         <v>6.99</v>
       </c>
-      <c r="K54" s="22">
-        <f t="shared" si="1"/>
+      <c r="K54" s="56">
+        <f t="shared" si="0"/>
         <v>41.94</v>
       </c>
       <c r="L54" s="27" t="s">
@@ -4189,8 +4175,8 @@
       <c r="J55" s="22">
         <v>5.99</v>
       </c>
-      <c r="K55" s="22">
-        <f t="shared" si="1"/>
+      <c r="K55" s="56">
+        <f t="shared" si="0"/>
         <v>23.96</v>
       </c>
       <c r="L55" s="27" t="s">
@@ -4229,8 +4215,8 @@
       <c r="J56" s="22">
         <v>5.99</v>
       </c>
-      <c r="K56" s="22">
-        <f t="shared" si="1"/>
+      <c r="K56" s="56">
+        <f t="shared" si="0"/>
         <v>17.97</v>
       </c>
       <c r="L56" s="27" t="s">
@@ -4269,8 +4255,8 @@
       <c r="J57" s="22">
         <v>5.99</v>
       </c>
-      <c r="K57" s="22">
-        <f t="shared" si="1"/>
+      <c r="K57" s="56">
+        <f t="shared" si="0"/>
         <v>35.94</v>
       </c>
       <c r="L57" s="27" t="s">
@@ -4309,8 +4295,8 @@
       <c r="J58" s="22">
         <v>1.49</v>
       </c>
-      <c r="K58" s="22">
-        <f t="shared" si="1"/>
+      <c r="K58" s="56">
+        <f t="shared" si="0"/>
         <v>5.96</v>
       </c>
       <c r="L58" s="27" t="s">
@@ -4349,9 +4335,9 @@
       <c r="J59" s="22">
         <v>5.99</v>
       </c>
-      <c r="K59" s="115">
-        <f t="shared" si="1"/>
-        <v>11.98</v>
+      <c r="K59" s="56">
+        <f t="shared" si="0"/>
+        <v>23.96</v>
       </c>
       <c r="L59" s="29" t="s">
         <v>201</v>
@@ -4389,8 +4375,8 @@
       <c r="J60" s="22">
         <v>2.09</v>
       </c>
-      <c r="K60" s="22">
-        <f>B60/D60*J60</f>
+      <c r="K60" s="56">
+        <f t="shared" si="0"/>
         <v>8.36</v>
       </c>
       <c r="L60" s="29" t="s">
@@ -4429,8 +4415,8 @@
       <c r="J61" s="22">
         <v>1.49</v>
       </c>
-      <c r="K61" s="22">
-        <f t="shared" ref="K61:K104" si="2">B61/D61*J61</f>
+      <c r="K61" s="56">
+        <f t="shared" si="0"/>
         <v>1.49</v>
       </c>
       <c r="L61" s="29" t="s">
@@ -4469,8 +4455,8 @@
       <c r="J62" s="22">
         <v>3.99</v>
       </c>
-      <c r="K62" s="22">
-        <f t="shared" si="2"/>
+      <c r="K62" s="56">
+        <f t="shared" si="0"/>
         <v>71.820000000000007</v>
       </c>
       <c r="L62" s="27" t="s">
@@ -4509,8 +4495,8 @@
       <c r="J63" s="22">
         <v>5.99</v>
       </c>
-      <c r="K63" s="22">
-        <f t="shared" si="2"/>
+      <c r="K63" s="56">
+        <f t="shared" si="0"/>
         <v>11.98</v>
       </c>
       <c r="L63" s="27" t="s">
@@ -4549,9 +4535,9 @@
       <c r="J64" s="22">
         <v>2.39</v>
       </c>
-      <c r="K64" s="22">
-        <f t="shared" si="2"/>
-        <v>4.78</v>
+      <c r="K64" s="56">
+        <f t="shared" si="0"/>
+        <v>9.56</v>
       </c>
       <c r="L64" s="27" t="s">
         <v>215</v>
@@ -4589,8 +4575,8 @@
       <c r="J65" s="22">
         <v>4.99</v>
       </c>
-      <c r="K65" s="22">
-        <f t="shared" si="2"/>
+      <c r="K65" s="56">
+        <f t="shared" si="0"/>
         <v>19.96</v>
       </c>
       <c r="L65" s="27" t="s">
@@ -4629,8 +4615,8 @@
       <c r="J66" s="22">
         <v>9.99</v>
       </c>
-      <c r="K66" s="22">
-        <f t="shared" si="2"/>
+      <c r="K66" s="56">
+        <f t="shared" si="0"/>
         <v>19.98</v>
       </c>
       <c r="L66" s="27" t="s">
@@ -4669,8 +4655,8 @@
       <c r="J67" s="22">
         <v>5.99</v>
       </c>
-      <c r="K67" s="22">
-        <f t="shared" si="2"/>
+      <c r="K67" s="56">
+        <f t="shared" si="0"/>
         <v>35.94</v>
       </c>
       <c r="L67" s="27" t="s">
@@ -4709,8 +4695,8 @@
       <c r="J68" s="22">
         <v>3.69</v>
       </c>
-      <c r="K68" s="22">
-        <f t="shared" si="2"/>
+      <c r="K68" s="56">
+        <f t="shared" si="0"/>
         <v>14.76</v>
       </c>
       <c r="L68" s="27" t="s">
@@ -4749,8 +4735,8 @@
       <c r="J69" s="22">
         <v>7.99</v>
       </c>
-      <c r="K69" s="22">
-        <f t="shared" si="2"/>
+      <c r="K69" s="56">
+        <f t="shared" si="0"/>
         <v>31.96</v>
       </c>
       <c r="L69" s="27" t="s">
@@ -4789,8 +4775,8 @@
       <c r="J70" s="22">
         <v>4.49</v>
       </c>
-      <c r="K70" s="22">
-        <f t="shared" si="2"/>
+      <c r="K70" s="56">
+        <f t="shared" ref="K70:K106" si="1">B70*J70</f>
         <v>17.96</v>
       </c>
       <c r="L70" s="27" t="s">
@@ -4829,8 +4815,8 @@
       <c r="J71" s="22">
         <v>16.989999999999998</v>
       </c>
-      <c r="K71" s="22">
-        <f t="shared" si="2"/>
+      <c r="K71" s="56">
+        <f t="shared" si="1"/>
         <v>33.979999999999997</v>
       </c>
       <c r="L71" s="27" t="s">
@@ -4869,8 +4855,8 @@
       <c r="J72" s="22">
         <v>13.99</v>
       </c>
-      <c r="K72" s="22">
-        <f t="shared" si="2"/>
+      <c r="K72" s="56">
+        <f t="shared" si="1"/>
         <v>41.97</v>
       </c>
       <c r="L72" s="27" t="s">
@@ -4909,11 +4895,11 @@
       <c r="J73" s="22">
         <v>4.99</v>
       </c>
-      <c r="K73" s="22">
-        <f t="shared" si="2"/>
+      <c r="K73" s="56">
+        <f t="shared" si="1"/>
         <v>19.96</v>
       </c>
-      <c r="L73" s="107" t="s">
+      <c r="L73" s="106" t="s">
         <v>365</v>
       </c>
       <c r="M73" s="9"/>
@@ -4949,8 +4935,8 @@
       <c r="J74" s="22">
         <v>7.99</v>
       </c>
-      <c r="K74" s="22">
-        <f t="shared" si="2"/>
+      <c r="K74" s="56">
+        <f t="shared" si="1"/>
         <v>15.98</v>
       </c>
       <c r="L74" s="27" t="s">
@@ -4990,9 +4976,9 @@
       <c r="J75" s="22">
         <v>3.99</v>
       </c>
-      <c r="K75" s="22">
-        <f t="shared" si="2"/>
-        <v>29.925000000000001</v>
+      <c r="K75" s="56">
+        <f t="shared" si="1"/>
+        <v>59.85</v>
       </c>
       <c r="L75" s="27" t="s">
         <v>243</v>
@@ -5030,8 +5016,8 @@
       <c r="J76" s="22">
         <v>2.79</v>
       </c>
-      <c r="K76" s="22">
-        <f t="shared" si="2"/>
+      <c r="K76" s="56">
+        <f t="shared" si="1"/>
         <v>22.32</v>
       </c>
       <c r="L76" s="27" t="s">
@@ -5070,8 +5056,8 @@
       <c r="J77" s="22">
         <v>1.29</v>
       </c>
-      <c r="K77" s="22">
-        <f t="shared" si="2"/>
+      <c r="K77" s="56">
+        <f t="shared" si="1"/>
         <v>1.29</v>
       </c>
       <c r="L77" s="27" t="s">
@@ -5110,8 +5096,8 @@
       <c r="J78" s="22">
         <v>3.99</v>
       </c>
-      <c r="K78" s="22">
-        <f t="shared" si="2"/>
+      <c r="K78" s="56">
+        <f t="shared" si="1"/>
         <v>15.96</v>
       </c>
       <c r="L78" s="29" t="s">
@@ -5150,9 +5136,9 @@
       <c r="J79" s="22">
         <v>1.79</v>
       </c>
-      <c r="K79" s="22">
-        <f t="shared" si="2"/>
-        <v>2.2374999999999998</v>
+      <c r="K79" s="56">
+        <f t="shared" si="1"/>
+        <v>8.9499999999999993</v>
       </c>
       <c r="L79" s="29" t="s">
         <v>255</v>
@@ -5187,8 +5173,8 @@
       <c r="J80" s="22">
         <v>6.8</v>
       </c>
-      <c r="K80" s="22">
-        <f t="shared" si="2"/>
+      <c r="K80" s="56">
+        <f t="shared" si="1"/>
         <v>27.2</v>
       </c>
       <c r="L80" s="27" t="s">
@@ -5211,7 +5197,7 @@
       <c r="E81" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="F81" s="72" t="s">
+      <c r="F81" s="37" t="s">
         <v>260</v>
       </c>
       <c r="G81" s="41" t="s">
@@ -5221,11 +5207,11 @@
         <v>12</v>
       </c>
       <c r="I81" s="59"/>
-      <c r="J81" s="73">
+      <c r="J81" s="72">
         <v>55.5</v>
       </c>
-      <c r="K81" s="22">
-        <f t="shared" si="2"/>
+      <c r="K81" s="56">
+        <f t="shared" si="1"/>
         <v>222</v>
       </c>
       <c r="L81" s="27" t="s">
@@ -5261,8 +5247,8 @@
       <c r="J82" s="22">
         <v>6.32</v>
       </c>
-      <c r="K82" s="22">
-        <f t="shared" si="2"/>
+      <c r="K82" s="56">
+        <f t="shared" si="1"/>
         <v>6.32</v>
       </c>
       <c r="L82" s="29" t="s">
@@ -5299,8 +5285,8 @@
       <c r="J83" s="22">
         <v>6.14</v>
       </c>
-      <c r="K83" s="22">
-        <f t="shared" si="2"/>
+      <c r="K83" s="56">
+        <f t="shared" si="1"/>
         <v>6.14</v>
       </c>
       <c r="L83" s="29" t="s">
@@ -5336,8 +5322,8 @@
       <c r="J84" s="22">
         <v>4.95</v>
       </c>
-      <c r="K84" s="22">
-        <f t="shared" si="2"/>
+      <c r="K84" s="56">
+        <f t="shared" si="1"/>
         <v>4.95</v>
       </c>
       <c r="L84" s="39" t="s">
@@ -5373,8 +5359,8 @@
       <c r="J85" s="22">
         <v>4.95</v>
       </c>
-      <c r="K85" s="22">
-        <f t="shared" si="2"/>
+      <c r="K85" s="56">
+        <f t="shared" si="1"/>
         <v>4.95</v>
       </c>
       <c r="L85" s="39" t="s">
@@ -5410,8 +5396,8 @@
       <c r="J86" s="22">
         <v>4.95</v>
       </c>
-      <c r="K86" s="22">
-        <f t="shared" si="2"/>
+      <c r="K86" s="56">
+        <f t="shared" si="1"/>
         <v>4.95</v>
       </c>
       <c r="L86" s="39" t="s">
@@ -5448,8 +5434,8 @@
       <c r="J87" s="22">
         <v>4.95</v>
       </c>
-      <c r="K87" s="22">
-        <f t="shared" si="2"/>
+      <c r="K87" s="56">
+        <f t="shared" si="1"/>
         <v>4.95</v>
       </c>
       <c r="L87" s="39" t="s">
@@ -5457,7 +5443,7 @@
       </c>
     </row>
     <row r="88" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="74" t="s">
+      <c r="A88" s="73" t="s">
         <v>279</v>
       </c>
       <c r="B88" s="39">
@@ -5473,7 +5459,7 @@
         <v>15</v>
       </c>
       <c r="F88" s="39"/>
-      <c r="G88" s="103" t="s">
+      <c r="G88" s="102" t="s">
         <v>280</v>
       </c>
       <c r="H88" s="39" t="s">
@@ -5483,16 +5469,16 @@
       <c r="J88" s="22">
         <v>0.36699999999999999</v>
       </c>
-      <c r="K88" s="22">
-        <f t="shared" si="2"/>
+      <c r="K88" s="56">
+        <f t="shared" si="1"/>
         <v>3.67</v>
       </c>
-      <c r="L88" s="75" t="s">
+      <c r="L88" s="74" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="76" t="s">
+      <c r="A89" s="75" t="s">
         <v>282</v>
       </c>
       <c r="B89" s="70">
@@ -5508,92 +5494,92 @@
         <v>15</v>
       </c>
       <c r="F89" s="70"/>
-      <c r="G89" s="104" t="s">
+      <c r="G89" s="103" t="s">
         <v>283</v>
       </c>
       <c r="H89" s="70" t="s">
         <v>12</v>
       </c>
       <c r="I89" s="71"/>
-      <c r="J89" s="77">
+      <c r="J89" s="76">
         <v>0.04</v>
       </c>
-      <c r="K89" s="77">
-        <f t="shared" si="2"/>
+      <c r="K89" s="56">
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="L89" s="78" t="s">
+      <c r="L89" s="77" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="79" t="s">
+      <c r="A90" s="78" t="s">
         <v>285</v>
       </c>
-      <c r="B90" s="80">
+      <c r="B90" s="79">
         <v>0</v>
       </c>
-      <c r="C90" s="80">
-        <v>1</v>
-      </c>
-      <c r="D90" s="80">
-        <v>1</v>
-      </c>
-      <c r="E90" s="80" t="s">
+      <c r="C90" s="79">
+        <v>1</v>
+      </c>
+      <c r="D90" s="79">
+        <v>1</v>
+      </c>
+      <c r="E90" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="F90" s="80"/>
-      <c r="G90" s="81"/>
-      <c r="H90" s="80" t="s">
+      <c r="F90" s="79"/>
+      <c r="G90" s="80"/>
+      <c r="H90" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="I90" s="82"/>
-      <c r="J90" s="83">
+      <c r="I90" s="81"/>
+      <c r="J90" s="82">
         <v>12.99</v>
       </c>
-      <c r="K90" s="83">
-        <f t="shared" si="2"/>
+      <c r="K90" s="56">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L90" s="80" t="s">
+      <c r="L90" s="79" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="79" t="s">
+      <c r="A91" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="B91" s="80">
+      <c r="B91" s="79">
         <v>0</v>
       </c>
-      <c r="C91" s="80">
-        <v>1</v>
-      </c>
-      <c r="D91" s="80">
-        <v>1</v>
-      </c>
-      <c r="E91" s="80" t="s">
+      <c r="C91" s="79">
+        <v>1</v>
+      </c>
+      <c r="D91" s="79">
+        <v>1</v>
+      </c>
+      <c r="E91" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="F91" s="80"/>
-      <c r="G91" s="81"/>
-      <c r="H91" s="80" t="s">
+      <c r="F91" s="79"/>
+      <c r="G91" s="80"/>
+      <c r="H91" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="I91" s="82"/>
-      <c r="J91" s="83">
+      <c r="I91" s="81"/>
+      <c r="J91" s="82">
         <v>25.99</v>
       </c>
-      <c r="K91" s="83">
-        <f t="shared" si="2"/>
+      <c r="K91" s="56">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L91" s="84" t="s">
+      <c r="L91" s="83" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="85" t="s">
+      <c r="A92" s="84" t="s">
         <v>289</v>
       </c>
       <c r="B92" s="70">
@@ -5609,26 +5595,26 @@
         <v>11</v>
       </c>
       <c r="F92" s="70"/>
-      <c r="G92" s="86" t="s">
+      <c r="G92" s="85" t="s">
         <v>290</v>
       </c>
       <c r="H92" s="70" t="s">
         <v>12</v>
       </c>
       <c r="I92" s="71"/>
-      <c r="J92" s="77">
+      <c r="J92" s="76">
         <v>7.99</v>
       </c>
-      <c r="K92" s="77">
-        <f t="shared" si="2"/>
+      <c r="K92" s="56">
+        <f t="shared" si="1"/>
         <v>7.99</v>
       </c>
-      <c r="L92" s="87" t="s">
+      <c r="L92" s="86" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="85" t="s">
+      <c r="A93" s="84" t="s">
         <v>292</v>
       </c>
       <c r="B93" s="70">
@@ -5644,26 +5630,26 @@
         <v>15</v>
       </c>
       <c r="F93" s="70"/>
-      <c r="G93" s="86" t="s">
+      <c r="G93" s="85" t="s">
         <v>293</v>
       </c>
       <c r="H93" s="70" t="s">
         <v>12</v>
       </c>
       <c r="I93" s="71"/>
-      <c r="J93" s="77">
+      <c r="J93" s="76">
         <v>15.59</v>
       </c>
-      <c r="K93" s="77">
-        <f t="shared" si="2"/>
+      <c r="K93" s="56">
+        <f t="shared" si="1"/>
         <v>15.59</v>
       </c>
-      <c r="L93" s="87" t="s">
+      <c r="L93" s="86" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="85" t="s">
+      <c r="A94" s="84" t="s">
         <v>295</v>
       </c>
       <c r="B94" s="70">
@@ -5679,26 +5665,26 @@
         <v>15</v>
       </c>
       <c r="F94" s="70"/>
-      <c r="G94" s="86" t="s">
+      <c r="G94" s="85" t="s">
         <v>296</v>
       </c>
       <c r="H94" s="70" t="s">
         <v>12</v>
       </c>
       <c r="I94" s="71"/>
-      <c r="J94" s="77">
+      <c r="J94" s="76">
         <v>12.56</v>
       </c>
-      <c r="K94" s="77">
-        <f t="shared" si="2"/>
+      <c r="K94" s="56">
+        <f t="shared" si="1"/>
         <v>12.56</v>
       </c>
-      <c r="L94" s="88" t="s">
+      <c r="L94" s="87" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="85" t="s">
+      <c r="A95" s="84" t="s">
         <v>298</v>
       </c>
       <c r="B95" s="70">
@@ -5714,26 +5700,26 @@
         <v>15</v>
       </c>
       <c r="F95" s="70"/>
-      <c r="G95" s="86" t="s">
+      <c r="G95" s="85" t="s">
         <v>299</v>
       </c>
       <c r="H95" s="70" t="s">
         <v>12</v>
       </c>
       <c r="I95" s="71"/>
-      <c r="J95" s="77">
+      <c r="J95" s="76">
         <v>15.59</v>
       </c>
-      <c r="K95" s="77">
-        <f t="shared" si="2"/>
+      <c r="K95" s="56">
+        <f t="shared" si="1"/>
         <v>15.59</v>
       </c>
-      <c r="L95" s="87" t="s">
+      <c r="L95" s="86" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="85" t="s">
+      <c r="A96" s="84" t="s">
         <v>301</v>
       </c>
       <c r="B96" s="70">
@@ -5749,21 +5735,21 @@
         <v>15</v>
       </c>
       <c r="F96" s="70"/>
-      <c r="G96" s="86" t="s">
+      <c r="G96" s="85" t="s">
         <v>302</v>
       </c>
       <c r="H96" s="70" t="s">
         <v>12</v>
       </c>
       <c r="I96" s="71"/>
-      <c r="J96" s="77">
+      <c r="J96" s="76">
         <v>15.59</v>
       </c>
-      <c r="K96" s="77">
-        <f t="shared" si="2"/>
+      <c r="K96" s="56">
+        <f t="shared" si="1"/>
         <v>15.59</v>
       </c>
-      <c r="L96" s="87" t="s">
+      <c r="L96" s="86" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5790,12 +5776,12 @@
       <c r="H97" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="I97" s="89"/>
+      <c r="I97" s="88"/>
       <c r="J97" s="64">
         <v>3.95</v>
       </c>
-      <c r="K97" s="64">
-        <f t="shared" si="2"/>
+      <c r="K97" s="56">
+        <f t="shared" si="1"/>
         <v>19.75</v>
       </c>
       <c r="L97" s="67" t="s">
@@ -5803,106 +5789,108 @@
       </c>
     </row>
     <row r="98" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="90" t="s">
+      <c r="A98" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="B98" s="91">
+      <c r="B98" s="90">
         <v>10</v>
       </c>
-      <c r="C98" s="91">
+      <c r="C98" s="90">
         <v>5</v>
       </c>
-      <c r="D98" s="91">
-        <v>1</v>
-      </c>
-      <c r="E98" s="91" t="s">
+      <c r="D98" s="90">
+        <v>1</v>
+      </c>
+      <c r="E98" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="F98" s="91"/>
+      <c r="F98" s="90"/>
       <c r="G98" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="H98" s="91" t="s">
+      <c r="H98" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="I98" s="92"/>
-      <c r="J98" s="93">
+      <c r="I98" s="91"/>
+      <c r="J98" s="92">
         <v>0.59</v>
       </c>
-      <c r="K98" s="93">
-        <f t="shared" si="2"/>
+      <c r="K98" s="56">
+        <f t="shared" si="1"/>
         <v>5.8999999999999995</v>
       </c>
-      <c r="L98" s="94" t="s">
+      <c r="L98" s="93" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="90" t="s">
+      <c r="A99" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="B99" s="91">
+      <c r="B99" s="90">
         <v>20</v>
       </c>
-      <c r="C99" s="91"/>
-      <c r="D99" s="91">
-        <v>1</v>
-      </c>
-      <c r="E99" s="91" t="s">
+      <c r="C99" s="90">
+        <v>20</v>
+      </c>
+      <c r="D99" s="90">
+        <v>1</v>
+      </c>
+      <c r="E99" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="F99" s="91" t="s">
+      <c r="F99" s="90" t="s">
         <v>19</v>
       </c>
       <c r="G99" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="H99" s="91" t="s">
+      <c r="H99" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="I99" s="92"/>
-      <c r="J99" s="93">
+      <c r="I99" s="91"/>
+      <c r="J99" s="92">
         <v>0.35</v>
       </c>
-      <c r="K99" s="93">
-        <f t="shared" si="2"/>
+      <c r="K99" s="56">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="L99" s="91" t="s">
+      <c r="L99" s="90" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="100" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="90" t="s">
+      <c r="A100" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="B100" s="91">
-        <v>1</v>
-      </c>
-      <c r="C100" s="91">
-        <v>1</v>
-      </c>
-      <c r="D100" s="91">
-        <v>1</v>
-      </c>
-      <c r="E100" s="91" t="s">
+      <c r="B100" s="90">
+        <v>1</v>
+      </c>
+      <c r="C100" s="90">
+        <v>1</v>
+      </c>
+      <c r="D100" s="90">
+        <v>1</v>
+      </c>
+      <c r="E100" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="F100" s="91" t="s">
+      <c r="F100" s="90" t="s">
         <v>13</v>
       </c>
       <c r="G100" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="H100" s="91" t="s">
+      <c r="H100" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="I100" s="92"/>
-      <c r="J100" s="93">
+      <c r="I100" s="91"/>
+      <c r="J100" s="92">
         <v>20.2</v>
       </c>
-      <c r="K100" s="93">
-        <f t="shared" si="2"/>
+      <c r="K100" s="56">
+        <f t="shared" si="1"/>
         <v>20.2</v>
       </c>
       <c r="L100" s="65" t="s">
@@ -5910,36 +5898,36 @@
       </c>
     </row>
     <row r="101" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="90" t="s">
+      <c r="A101" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="B101" s="91">
-        <v>1</v>
-      </c>
-      <c r="C101" s="91">
-        <v>1</v>
-      </c>
-      <c r="D101" s="91">
-        <v>1</v>
-      </c>
-      <c r="E101" s="91" t="s">
+      <c r="B101" s="90">
+        <v>1</v>
+      </c>
+      <c r="C101" s="90">
+        <v>1</v>
+      </c>
+      <c r="D101" s="90">
+        <v>1</v>
+      </c>
+      <c r="E101" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="F101" s="91" t="s">
+      <c r="F101" s="90" t="s">
         <v>26</v>
       </c>
       <c r="G101" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="H101" s="91" t="s">
+      <c r="H101" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="I101" s="92"/>
-      <c r="J101" s="93">
+      <c r="I101" s="91"/>
+      <c r="J101" s="92">
         <v>19.649999999999999</v>
       </c>
-      <c r="K101" s="93">
-        <f t="shared" si="2"/>
+      <c r="K101" s="56">
+        <f t="shared" si="1"/>
         <v>19.649999999999999</v>
       </c>
       <c r="L101" s="65" t="s">
@@ -5947,35 +5935,35 @@
       </c>
     </row>
     <row r="102" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="95" t="s">
+      <c r="A102" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="B102" s="96">
+      <c r="B102" s="95">
         <v>5</v>
       </c>
-      <c r="C102" s="96">
+      <c r="C102" s="95">
         <v>5</v>
       </c>
-      <c r="D102" s="91">
+      <c r="D102" s="90">
         <v>1</v>
       </c>
       <c r="E102" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="F102" s="96"/>
-      <c r="G102" s="97"/>
+      <c r="F102" s="95"/>
+      <c r="G102" s="96"/>
       <c r="H102" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="I102" s="98"/>
-      <c r="J102" s="125">
+      <c r="I102" s="97"/>
+      <c r="J102" s="116">
         <v>5.99</v>
       </c>
-      <c r="K102" s="93">
-        <f t="shared" si="2"/>
+      <c r="K102" s="56">
+        <f t="shared" si="1"/>
         <v>29.950000000000003</v>
       </c>
-      <c r="L102" s="99" t="s">
+      <c r="L102" s="98" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5998,7 +5986,7 @@
       <c r="F103" s="40" t="s">
         <v>316</v>
       </c>
-      <c r="G103" s="105" t="s">
+      <c r="G103" s="104" t="s">
         <v>339</v>
       </c>
       <c r="H103" s="47" t="s">
@@ -6010,11 +5998,11 @@
       <c r="J103" s="32">
         <v>3.78</v>
       </c>
-      <c r="K103" s="32">
-        <f t="shared" si="2"/>
-        <v>0.1512</v>
-      </c>
-      <c r="L103" s="100" t="s">
+      <c r="K103" s="56">
+        <f t="shared" si="1"/>
+        <v>3.78</v>
+      </c>
+      <c r="L103" s="99" t="s">
         <v>338</v>
       </c>
     </row>
@@ -6049,11 +6037,11 @@
       <c r="J104" s="32">
         <v>0.96</v>
       </c>
-      <c r="K104" s="32">
-        <f t="shared" si="2"/>
+      <c r="K104" s="56">
+        <f t="shared" si="1"/>
         <v>3.84</v>
       </c>
-      <c r="L104" s="100" t="s">
+      <c r="L104" s="99" t="s">
         <v>317</v>
       </c>
     </row>
@@ -6076,19 +6064,19 @@
       <c r="F105" s="40" t="s">
         <v>344</v>
       </c>
-      <c r="G105" s="101"/>
+      <c r="G105" s="100"/>
       <c r="H105" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="I105" s="102"/>
+      <c r="I105" s="101"/>
       <c r="J105" s="32">
         <v>11.75</v>
       </c>
-      <c r="K105" s="32">
-        <f>B105/D105*J105</f>
+      <c r="K105" s="56">
+        <f t="shared" si="1"/>
         <v>11.75</v>
       </c>
-      <c r="L105" s="100" t="s">
+      <c r="L105" s="99" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6111,19 +6099,19 @@
       <c r="F106" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="G106" s="101"/>
+      <c r="G106" s="100"/>
       <c r="H106" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="I106" s="102"/>
+      <c r="I106" s="101"/>
       <c r="J106" s="32">
         <v>15.25</v>
       </c>
-      <c r="K106" s="32">
-        <f>B106/D106*J106</f>
+      <c r="K106" s="56">
+        <f t="shared" si="1"/>
         <v>15.25</v>
       </c>
-      <c r="L106" s="100" t="s">
+      <c r="L106" s="99" t="s">
         <v>345</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Closes #41 by increasing hole size on serial splitter board to be 4-40 thru holes, updating the part used for the 5V regulator (previous part was incorrect part number), and updating corresponding mounting pattern. Made changes in the CAD assembly as well as updating the .DXF file for laser cutting
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\JPL Open Source Rover\open-source-rover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\open-source-rover\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2009,8 +2009,8 @@
   <dimension ref="A1:AA970"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L50" sqref="L50"/>
+      <pane ySplit="4" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updated link for 0.5" collar clamps
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cox/Documents/open source rover/osr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7F4A3B-29EC-B744-BB75-9FB098DEBA74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ECEBFA-672B-4342-96F7-6ECD47783B6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57180" yWindow="2360" windowWidth="33600" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,9 +415,6 @@
     <t>6157K14</t>
   </si>
   <si>
-    <t>.5”D Collared Clamp</t>
-  </si>
-  <si>
     <t>1 Inch PVC</t>
   </si>
   <si>
@@ -1118,6 +1115,9 @@
   </si>
   <si>
     <t>https://www.pololu.com/product/3256</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/6157k14</t>
   </si>
 </sst>
 </file>
@@ -2010,8 +2010,8 @@
   <dimension ref="A1:AA970"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2035,7 +2035,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="109" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="123" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B1" s="124"/>
       <c r="C1" s="124"/>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="2" spans="1:27" s="111" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="127" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B2" s="127"/>
       <c r="C2" s="127"/>
@@ -2062,17 +2062,17 @@
       <c r="H2" s="114"/>
       <c r="I2" s="114"/>
       <c r="J2" s="119" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K2" s="120">
         <f>SUM(K5:K150)</f>
-        <v>2496.3000000000002</v>
+        <v>2501.36</v>
       </c>
       <c r="L2" s="114"/>
     </row>
     <row r="3" spans="1:27" s="111" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="115" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B3" s="115"/>
       <c r="C3" s="115"/>
@@ -2110,7 +2110,7 @@
         <v>6</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>7</v>
@@ -2445,7 +2445,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J12" s="23">
         <v>9.25</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="17" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B17" s="39">
         <v>25</v>
@@ -2634,7 +2634,7 @@
         <v>74</v>
       </c>
       <c r="G17" s="116" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H17" s="39" t="s">
         <v>12</v>
@@ -2648,13 +2648,13 @@
         <v>0.72</v>
       </c>
       <c r="L17" s="117" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B18" s="39">
         <v>25</v>
@@ -2672,7 +2672,7 @@
         <v>53</v>
       </c>
       <c r="G18" s="116" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H18" s="39" t="s">
         <v>12</v>
@@ -2686,7 +2686,7 @@
         <v>0.72</v>
       </c>
       <c r="L18" s="110" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M18" s="9"/>
     </row>
@@ -2762,7 +2762,7 @@
         <v>4.49</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M20" s="9"/>
     </row>
@@ -2792,7 +2792,7 @@
         <v>58</v>
       </c>
       <c r="I21" s="61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J21" s="23">
         <v>25.27</v>
@@ -2832,7 +2832,7 @@
         <v>58</v>
       </c>
       <c r="I22" s="61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J22" s="23">
         <v>12.9</v>
@@ -2872,7 +2872,7 @@
         <v>58</v>
       </c>
       <c r="I23" s="61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J23" s="23">
         <f>38.9+36.9</f>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="24" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B24" s="39">
         <v>300</v>
@@ -2914,7 +2914,7 @@
         <v>93</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J24" s="23">
         <v>3.45</v>
@@ -2954,7 +2954,7 @@
         <v>93</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J25" s="23">
         <v>5.61</v>
@@ -2998,7 +2998,7 @@
         <v>93</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J26" s="23">
         <v>2.72</v>
@@ -3041,7 +3041,7 @@
         <v>93</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J27" s="23">
         <v>2.79</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="28" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B28" s="39">
         <v>100</v>
@@ -3085,7 +3085,7 @@
         <v>93</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J28" s="23">
         <v>3.72</v>
@@ -3095,7 +3095,7 @@
         <v>3.72</v>
       </c>
       <c r="L28" s="27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M28" s="9"/>
       <c r="Y28" s="9"/>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B29" s="39">
         <v>100</v>
@@ -3128,7 +3128,7 @@
         <v>93</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J29" s="23">
         <v>3.72</v>
@@ -3138,7 +3138,7 @@
         <v>3.72</v>
       </c>
       <c r="L29" s="27" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M29" s="9"/>
       <c r="Y29" s="9"/>
@@ -3147,7 +3147,7 @@
     </row>
     <row r="30" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B30" s="41">
         <v>100</v>
@@ -3171,7 +3171,7 @@
         <v>93</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J30" s="23">
         <v>4.07</v>
@@ -3181,13 +3181,13 @@
         <v>4.07</v>
       </c>
       <c r="L30" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B31" s="41">
         <v>100</v>
@@ -3211,7 +3211,7 @@
         <v>93</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J31" s="23">
         <v>4.41</v>
@@ -3221,13 +3221,13 @@
         <v>4.41</v>
       </c>
       <c r="L31" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M31" s="9"/>
     </row>
     <row r="32" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B32" s="41">
         <v>50</v>
@@ -3251,7 +3251,7 @@
         <v>93</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J32" s="23">
         <v>5.42</v>
@@ -3261,13 +3261,13 @@
         <v>5.42</v>
       </c>
       <c r="L32" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M32" s="9"/>
     </row>
     <row r="33" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B33" s="39">
         <v>50</v>
@@ -3291,7 +3291,7 @@
         <v>93</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J33" s="23">
         <v>6.51</v>
@@ -3301,13 +3301,13 @@
         <v>6.51</v>
       </c>
       <c r="L33" s="27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M33" s="9"/>
     </row>
     <row r="34" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B34" s="39">
         <v>100</v>
@@ -3331,7 +3331,7 @@
         <v>93</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J34" s="23">
         <v>2.87</v>
@@ -3347,7 +3347,7 @@
     </row>
     <row r="35" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B35" s="41">
         <v>100</v>
@@ -3371,7 +3371,7 @@
         <v>93</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J35" s="23">
         <v>7.7</v>
@@ -3381,7 +3381,7 @@
         <v>7.7</v>
       </c>
       <c r="L35" s="26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -3405,13 +3405,13 @@
         <v>126</v>
       </c>
       <c r="G36" s="43" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H36" s="39" t="s">
         <v>58</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J36" s="23">
         <v>23.16</v>
@@ -3421,7 +3421,7 @@
         <v>23.16</v>
       </c>
       <c r="L36" s="110" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -3451,23 +3451,23 @@
         <v>58</v>
       </c>
       <c r="I37" s="61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J37" s="23">
-        <v>2.2599999999999998</v>
+        <v>2.72</v>
       </c>
       <c r="K37" s="23">
         <f t="shared" si="1"/>
-        <v>24.86</v>
-      </c>
-      <c r="L37" s="28" t="s">
-        <v>130</v>
+        <v>29.92</v>
+      </c>
+      <c r="L37" s="110" t="s">
+        <v>364</v>
       </c>
       <c r="M37" s="9"/>
     </row>
     <row r="38" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="39">
         <v>1</v>
@@ -3482,16 +3482,16 @@
         <v>90</v>
       </c>
       <c r="F38" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" s="43" t="s">
         <v>132</v>
-      </c>
-      <c r="G38" s="43" t="s">
-        <v>133</v>
       </c>
       <c r="H38" s="60" t="s">
         <v>58</v>
       </c>
       <c r="I38" s="61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J38" s="23">
         <v>4.92</v>
@@ -3501,13 +3501,13 @@
         <v>4.92</v>
       </c>
       <c r="L38" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M38" s="9"/>
     </row>
     <row r="39" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B39" s="41">
         <v>68</v>
@@ -3522,16 +3522,16 @@
         <v>90</v>
       </c>
       <c r="F39" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="45" t="s">
         <v>136</v>
-      </c>
-      <c r="G39" s="45" t="s">
-        <v>137</v>
       </c>
       <c r="H39" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J39" s="23">
         <v>0.23</v>
@@ -3541,13 +3541,13 @@
         <v>15.64</v>
       </c>
       <c r="L39" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M39" s="9"/>
     </row>
     <row r="40" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B40" s="39">
         <v>4</v>
@@ -3562,16 +3562,16 @@
         <v>90</v>
       </c>
       <c r="F40" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G40" s="46" t="s">
         <v>140</v>
-      </c>
-      <c r="G40" s="46" t="s">
-        <v>141</v>
       </c>
       <c r="H40" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J40" s="23">
         <v>0.3</v>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="41" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B41" s="41">
         <v>10</v>
@@ -3603,16 +3603,16 @@
         <v>90</v>
       </c>
       <c r="F41" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="G41" s="45" t="s">
         <v>143</v>
-      </c>
-      <c r="G41" s="45" t="s">
-        <v>144</v>
       </c>
       <c r="H41" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J41" s="23">
         <v>0.23</v>
@@ -3622,13 +3622,13 @@
         <v>2.3000000000000003</v>
       </c>
       <c r="L41" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M41" s="9"/>
     </row>
     <row r="42" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B42" s="41">
         <v>15</v>
@@ -3643,16 +3643,16 @@
         <v>90</v>
       </c>
       <c r="F42" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="G42" s="45" t="s">
         <v>147</v>
-      </c>
-      <c r="G42" s="45" t="s">
-        <v>148</v>
       </c>
       <c r="H42" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J42" s="23">
         <v>0.27</v>
@@ -3662,7 +3662,7 @@
         <v>4.0500000000000007</v>
       </c>
       <c r="L42" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M42" s="9"/>
       <c r="Y42" s="9"/>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="43" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B43" s="39">
         <v>10</v>
@@ -3686,16 +3686,16 @@
         <v>90</v>
       </c>
       <c r="F43" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="45" t="s">
         <v>151</v>
-      </c>
-      <c r="G43" s="45" t="s">
-        <v>152</v>
       </c>
       <c r="H43" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J43" s="23">
         <v>0.37</v>
@@ -3705,7 +3705,7 @@
         <v>3.7</v>
       </c>
       <c r="L43" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M43" s="9"/>
       <c r="Y43" s="9"/>
@@ -3714,7 +3714,7 @@
     </row>
     <row r="44" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B44" s="41">
         <v>10</v>
@@ -3729,16 +3729,16 @@
         <v>90</v>
       </c>
       <c r="F44" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="G44" s="47" t="s">
         <v>155</v>
-      </c>
-      <c r="G44" s="47" t="s">
-        <v>156</v>
       </c>
       <c r="H44" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J44" s="23">
         <v>0.48</v>
@@ -3748,7 +3748,7 @@
         <v>4.8</v>
       </c>
       <c r="L44" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M44" s="9"/>
       <c r="Y44" s="9"/>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="45" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B45" s="39">
         <v>100</v>
@@ -3772,16 +3772,16 @@
         <v>90</v>
       </c>
       <c r="F45" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G45" s="45" t="s">
         <v>159</v>
-      </c>
-      <c r="G45" s="45" t="s">
-        <v>160</v>
       </c>
       <c r="H45" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J45" s="23">
         <v>1.17</v>
@@ -3791,7 +3791,7 @@
         <v>1.17</v>
       </c>
       <c r="L45" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M45" s="9"/>
       <c r="Y45" s="9"/>
@@ -3800,7 +3800,7 @@
     </row>
     <row r="46" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B46" s="41">
         <v>100</v>
@@ -3815,16 +3815,16 @@
         <v>90</v>
       </c>
       <c r="F46" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="G46" s="45" t="s">
         <v>163</v>
-      </c>
-      <c r="G46" s="45" t="s">
-        <v>164</v>
       </c>
       <c r="H46" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J46" s="23">
         <v>1.4</v>
@@ -3834,13 +3834,13 @@
         <v>1.4</v>
       </c>
       <c r="L46" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M46" s="9"/>
     </row>
     <row r="47" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B47" s="39">
         <v>20</v>
@@ -3855,16 +3855,16 @@
         <v>90</v>
       </c>
       <c r="F47" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="G47" s="43" t="s">
         <v>167</v>
-      </c>
-      <c r="G47" s="43" t="s">
-        <v>168</v>
       </c>
       <c r="H47" s="39" t="s">
         <v>93</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J47" s="23">
         <v>2.4700000000000002</v>
@@ -3874,13 +3874,13 @@
         <v>9.8800000000000008</v>
       </c>
       <c r="L47" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M47" s="9"/>
     </row>
     <row r="48" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B48" s="39">
         <v>5</v>
@@ -3895,7 +3895,7 @@
         <v>110</v>
       </c>
       <c r="F48" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G48" s="43" t="s">
         <v>19</v>
@@ -3912,13 +3912,13 @@
         <v>349.75</v>
       </c>
       <c r="L48" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M48" s="9"/>
     </row>
     <row r="49" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B49" s="39">
         <v>1</v>
@@ -3933,7 +3933,7 @@
         <v>110</v>
       </c>
       <c r="F49" s="39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G49" s="43" t="s">
         <v>19</v>
@@ -3950,13 +3950,13 @@
         <v>14.95</v>
       </c>
       <c r="L49" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M49" s="9"/>
     </row>
     <row r="50" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B50" s="39">
         <v>6</v>
@@ -3988,7 +3988,7 @@
         <v>209.70000000000002</v>
       </c>
       <c r="L50" s="110" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M50" s="9">
         <v>0</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="51" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B51" s="39">
         <v>4</v>
@@ -4011,7 +4011,7 @@
         <v>110</v>
       </c>
       <c r="F51" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G51" s="43" t="s">
         <v>19</v>
@@ -4028,13 +4028,13 @@
         <v>79.8</v>
       </c>
       <c r="L51" s="110" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M51" s="9"/>
     </row>
     <row r="52" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B52" s="39">
         <v>6</v>
@@ -4046,10 +4046,10 @@
         <v>1</v>
       </c>
       <c r="E52" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="F52" s="39" t="s">
         <v>178</v>
-      </c>
-      <c r="F52" s="39" t="s">
-        <v>179</v>
       </c>
       <c r="G52" s="43">
         <v>585440</v>
@@ -4058,7 +4058,7 @@
         <v>58</v>
       </c>
       <c r="I52" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J52" s="23">
         <v>2.99</v>
@@ -4068,13 +4068,13 @@
         <v>17.940000000000001</v>
       </c>
       <c r="L52" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M52" s="9"/>
     </row>
     <row r="53" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B53" s="39">
         <v>8</v>
@@ -4086,10 +4086,10 @@
         <v>1</v>
       </c>
       <c r="E53" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F53" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G53" s="43">
         <v>535110</v>
@@ -4098,7 +4098,7 @@
         <v>58</v>
       </c>
       <c r="I53" s="61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J53" s="23">
         <v>5.99</v>
@@ -4108,13 +4108,13 @@
         <v>47.92</v>
       </c>
       <c r="L53" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M53" s="9"/>
     </row>
     <row r="54" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B54" s="39">
         <v>6</v>
@@ -4126,10 +4126,10 @@
         <v>1</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F54" s="39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G54" s="43">
         <v>535118</v>
@@ -4138,7 +4138,7 @@
         <v>58</v>
       </c>
       <c r="I54" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J54" s="23">
         <v>6.99</v>
@@ -4148,13 +4148,13 @@
         <v>41.94</v>
       </c>
       <c r="L54" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M54" s="9"/>
     </row>
     <row r="55" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B55" s="39">
         <v>4</v>
@@ -4166,10 +4166,10 @@
         <v>1</v>
       </c>
       <c r="E55" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F55" s="39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G55" s="48">
         <v>545588</v>
@@ -4178,7 +4178,7 @@
         <v>58</v>
       </c>
       <c r="I55" s="61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J55" s="23">
         <v>5.99</v>
@@ -4188,13 +4188,13 @@
         <v>23.96</v>
       </c>
       <c r="L55" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M55" s="9"/>
     </row>
     <row r="56" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B56" s="39">
         <v>3</v>
@@ -4206,10 +4206,10 @@
         <v>1</v>
       </c>
       <c r="E56" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F56" s="39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G56" s="43">
         <v>545600</v>
@@ -4218,7 +4218,7 @@
         <v>58</v>
       </c>
       <c r="I56" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J56" s="23">
         <v>5.99</v>
@@ -4228,13 +4228,13 @@
         <v>17.97</v>
       </c>
       <c r="L56" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M56" s="9"/>
     </row>
     <row r="57" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B57" s="39">
         <v>6</v>
@@ -4246,10 +4246,10 @@
         <v>1</v>
       </c>
       <c r="E57" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F57" s="39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G57" s="43">
         <v>545608</v>
@@ -4258,7 +4258,7 @@
         <v>58</v>
       </c>
       <c r="I57" s="61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J57" s="23">
         <v>5.99</v>
@@ -4268,13 +4268,13 @@
         <v>35.94</v>
       </c>
       <c r="L57" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M57" s="9"/>
     </row>
     <row r="58" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B58" s="39">
         <v>4</v>
@@ -4286,10 +4286,10 @@
         <v>1</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F58" s="39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G58" s="43">
         <v>634066</v>
@@ -4298,7 +4298,7 @@
         <v>58</v>
       </c>
       <c r="I58" s="61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J58" s="23">
         <v>1.49</v>
@@ -4308,13 +4308,13 @@
         <v>5.96</v>
       </c>
       <c r="L58" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M58" s="9"/>
     </row>
     <row r="59" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B59" s="41">
         <v>16</v>
@@ -4326,10 +4326,10 @@
         <v>2</v>
       </c>
       <c r="E59" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F59" s="41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G59" s="47">
         <v>585470</v>
@@ -4338,7 +4338,7 @@
         <v>58</v>
       </c>
       <c r="I59" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J59" s="23">
         <v>5.99</v>
@@ -4348,13 +4348,13 @@
         <v>47.92</v>
       </c>
       <c r="L59" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M59" s="9"/>
     </row>
     <row r="60" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B60" s="41">
         <v>4</v>
@@ -4366,10 +4366,10 @@
         <v>1</v>
       </c>
       <c r="E60" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F60" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G60" s="48">
         <v>635254</v>
@@ -4378,7 +4378,7 @@
         <v>58</v>
       </c>
       <c r="I60" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J60" s="23">
         <v>2.09</v>
@@ -4388,13 +4388,13 @@
         <v>8.36</v>
       </c>
       <c r="L60" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M60" s="9"/>
     </row>
     <row r="61" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B61" s="41">
         <v>1</v>
@@ -4406,10 +4406,10 @@
         <v>1</v>
       </c>
       <c r="E61" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F61" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G61" s="48">
         <v>635252</v>
@@ -4418,7 +4418,7 @@
         <v>58</v>
       </c>
       <c r="I61" s="25" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J61" s="23">
         <v>1.49</v>
@@ -4428,13 +4428,13 @@
         <v>1.49</v>
       </c>
       <c r="L61" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M61" s="9"/>
     </row>
     <row r="62" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B62" s="39">
         <v>18</v>
@@ -4446,10 +4446,10 @@
         <v>1</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F62" s="39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G62" s="43">
         <v>585442</v>
@@ -4458,7 +4458,7 @@
         <v>58</v>
       </c>
       <c r="I62" s="61" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J62" s="23">
         <v>3.99</v>
@@ -4468,13 +4468,13 @@
         <v>71.820000000000007</v>
       </c>
       <c r="L62" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M62" s="9"/>
     </row>
     <row r="63" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B63" s="39">
         <v>2</v>
@@ -4486,10 +4486,10 @@
         <v>1</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F63" s="39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G63" s="43">
         <v>585546</v>
@@ -4498,7 +4498,7 @@
         <v>58</v>
       </c>
       <c r="I63" s="61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J63" s="23">
         <v>5.99</v>
@@ -4508,13 +4508,13 @@
         <v>11.98</v>
       </c>
       <c r="L63" s="28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M63" s="9"/>
     </row>
     <row r="64" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B64" s="39">
         <v>8</v>
@@ -4526,10 +4526,10 @@
         <v>2</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F64" s="39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G64" s="43">
         <v>585404</v>
@@ -4538,7 +4538,7 @@
         <v>58</v>
       </c>
       <c r="I64" s="61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J64" s="23">
         <v>2.39</v>
@@ -4548,13 +4548,13 @@
         <v>9.56</v>
       </c>
       <c r="L64" s="28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M64" s="9"/>
     </row>
     <row r="65" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B65" s="39">
         <v>4</v>
@@ -4566,10 +4566,10 @@
         <v>1</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F65" s="39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G65" s="43">
         <v>625049</v>
@@ -4578,7 +4578,7 @@
         <v>58</v>
       </c>
       <c r="I65" s="61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J65" s="23">
         <v>4.99</v>
@@ -4588,13 +4588,13 @@
         <v>19.96</v>
       </c>
       <c r="L65" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M65" s="9"/>
     </row>
     <row r="66" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B66" s="39">
         <v>2</v>
@@ -4606,10 +4606,10 @@
         <v>1</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F66" s="39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G66" s="43">
         <v>545512</v>
@@ -4618,7 +4618,7 @@
         <v>58</v>
       </c>
       <c r="I66" s="61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J66" s="23">
         <v>9.99</v>
@@ -4628,13 +4628,13 @@
         <v>19.98</v>
       </c>
       <c r="L66" s="28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M66" s="9"/>
     </row>
     <row r="67" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B67" s="39">
         <v>6</v>
@@ -4646,10 +4646,10 @@
         <v>1</v>
       </c>
       <c r="E67" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F67" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G67" s="43">
         <v>545680</v>
@@ -4658,7 +4658,7 @@
         <v>58</v>
       </c>
       <c r="I67" s="61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J67" s="23">
         <v>5.99</v>
@@ -4668,13 +4668,13 @@
         <v>35.94</v>
       </c>
       <c r="L67" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M67" s="9"/>
     </row>
     <row r="68" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B68" s="39">
         <v>4</v>
@@ -4686,19 +4686,19 @@
         <v>1</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F68" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="G68" s="70" t="s">
         <v>221</v>
-      </c>
-      <c r="G68" s="70" t="s">
-        <v>222</v>
       </c>
       <c r="H68" s="60" t="s">
         <v>58</v>
       </c>
       <c r="I68" s="61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J68" s="23">
         <v>3.69</v>
@@ -4708,13 +4708,13 @@
         <v>14.76</v>
       </c>
       <c r="L68" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M68" s="9"/>
     </row>
     <row r="69" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B69" s="39">
         <v>4</v>
@@ -4726,10 +4726,10 @@
         <v>1</v>
       </c>
       <c r="E69" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F69" s="39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G69" s="70">
         <v>615362</v>
@@ -4738,7 +4738,7 @@
         <v>58</v>
       </c>
       <c r="I69" s="61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J69" s="23">
         <v>7.99</v>
@@ -4748,13 +4748,13 @@
         <v>31.96</v>
       </c>
       <c r="L69" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M69" s="9"/>
     </row>
     <row r="70" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B70" s="39">
         <v>4</v>
@@ -4766,10 +4766,10 @@
         <v>1</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F70" s="39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G70" s="43">
         <v>585443</v>
@@ -4778,7 +4778,7 @@
         <v>58</v>
       </c>
       <c r="I70" s="61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J70" s="23">
         <v>4.49</v>
@@ -4788,13 +4788,13 @@
         <v>17.96</v>
       </c>
       <c r="L70" s="28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M70" s="9"/>
     </row>
     <row r="71" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B71" s="39">
         <v>2</v>
@@ -4806,10 +4806,10 @@
         <v>1</v>
       </c>
       <c r="E71" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F71" s="39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G71" s="43">
         <v>585006</v>
@@ -4818,7 +4818,7 @@
         <v>58</v>
       </c>
       <c r="I71" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J71" s="23">
         <v>16.989999999999998</v>
@@ -4828,13 +4828,13 @@
         <v>33.979999999999997</v>
       </c>
       <c r="L71" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M71" s="9"/>
     </row>
     <row r="72" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B72" s="39">
         <v>3</v>
@@ -4846,10 +4846,10 @@
         <v>1</v>
       </c>
       <c r="E72" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F72" s="39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G72" s="71">
         <v>585004</v>
@@ -4858,7 +4858,7 @@
         <v>58</v>
       </c>
       <c r="I72" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J72" s="23">
         <v>13.99</v>
@@ -4868,13 +4868,13 @@
         <v>41.97</v>
       </c>
       <c r="L72" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M72" s="9"/>
     </row>
     <row r="73" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B73" s="41">
         <v>4</v>
@@ -4886,10 +4886,10 @@
         <v>1</v>
       </c>
       <c r="E73" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G73" s="47">
         <v>585444</v>
@@ -4898,7 +4898,7 @@
         <v>58</v>
       </c>
       <c r="I73" s="73" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J73" s="23">
         <v>4.99</v>
@@ -4908,13 +4908,13 @@
         <v>19.96</v>
       </c>
       <c r="L73" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M73" s="9"/>
     </row>
     <row r="74" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B74" s="39">
         <v>2</v>
@@ -4926,10 +4926,10 @@
         <v>1</v>
       </c>
       <c r="E74" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F74" s="39" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G74" s="43">
         <v>585450</v>
@@ -4938,7 +4938,7 @@
         <v>58</v>
       </c>
       <c r="I74" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J74" s="23">
         <v>7.99</v>
@@ -4948,13 +4948,13 @@
         <v>15.98</v>
       </c>
       <c r="L74" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M74" s="9"/>
     </row>
     <row r="75" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B75" s="39">
         <v>34</v>
@@ -4967,10 +4967,10 @@
         <v>2</v>
       </c>
       <c r="E75" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F75" s="39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G75" s="43">
         <v>545532</v>
@@ -4979,7 +4979,7 @@
         <v>58</v>
       </c>
       <c r="I75" s="61" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J75" s="23">
         <v>3.99</v>
@@ -4989,13 +4989,13 @@
         <v>67.83</v>
       </c>
       <c r="L75" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M75" s="9"/>
     </row>
     <row r="76" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B76" s="39">
         <v>8</v>
@@ -5007,10 +5007,10 @@
         <v>1</v>
       </c>
       <c r="E76" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F76" s="39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G76" s="43">
         <v>585592</v>
@@ -5019,7 +5019,7 @@
         <v>58</v>
       </c>
       <c r="I76" s="61" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J76" s="23">
         <v>2.79</v>
@@ -5029,13 +5029,13 @@
         <v>22.32</v>
       </c>
       <c r="L76" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M76" s="9"/>
     </row>
     <row r="77" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B77" s="39">
         <v>1</v>
@@ -5047,10 +5047,10 @@
         <v>1</v>
       </c>
       <c r="E77" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F77" s="39" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G77" s="43">
         <v>585468</v>
@@ -5059,7 +5059,7 @@
         <v>58</v>
       </c>
       <c r="I77" s="61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J77" s="23">
         <v>1.29</v>
@@ -5069,13 +5069,13 @@
         <v>1.29</v>
       </c>
       <c r="L77" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M77" s="9"/>
     </row>
     <row r="78" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B78" s="41">
         <v>4</v>
@@ -5087,10 +5087,10 @@
         <v>1</v>
       </c>
       <c r="E78" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F78" s="41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G78" s="47">
         <v>555104</v>
@@ -5099,7 +5099,7 @@
         <v>58</v>
       </c>
       <c r="I78" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J78" s="23">
         <v>3.99</v>
@@ -5109,13 +5109,13 @@
         <v>15.96</v>
       </c>
       <c r="L78" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M78" s="9"/>
     </row>
     <row r="79" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B79" s="41">
         <v>16</v>
@@ -5127,10 +5127,10 @@
         <v>4</v>
       </c>
       <c r="E79" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F79" s="41" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G79" s="48">
         <v>633126</v>
@@ -5139,7 +5139,7 @@
         <v>93</v>
       </c>
       <c r="I79" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J79" s="23">
         <v>1.79</v>
@@ -5149,12 +5149,12 @@
         <v>7.16</v>
       </c>
       <c r="L79" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B80" s="39">
         <v>4</v>
@@ -5166,13 +5166,13 @@
         <v>1</v>
       </c>
       <c r="E80" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="F80" s="39" t="s">
         <v>255</v>
       </c>
-      <c r="F80" s="39" t="s">
-        <v>256</v>
-      </c>
       <c r="G80" s="43" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H80" s="60" t="s">
         <v>12</v>
@@ -5186,12 +5186,12 @@
         <v>27.2</v>
       </c>
       <c r="L80" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B81" s="39">
         <v>4</v>
@@ -5203,13 +5203,13 @@
         <v>1</v>
       </c>
       <c r="E81" s="39" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F81" s="74" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G81" s="43" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H81" s="60" t="s">
         <v>12</v>
@@ -5223,12 +5223,12 @@
         <v>222</v>
       </c>
       <c r="L81" s="28" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B82" s="41">
         <v>1</v>
@@ -5246,7 +5246,7 @@
         <v>19</v>
       </c>
       <c r="G82" s="47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H82" s="41" t="s">
         <v>12</v>
@@ -5260,13 +5260,13 @@
         <v>6.32</v>
       </c>
       <c r="L82" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M82" s="15"/>
     </row>
     <row r="83" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B83" s="41">
         <v>1</v>
@@ -5284,7 +5284,7 @@
         <v>19</v>
       </c>
       <c r="G83" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H83" s="41" t="s">
         <v>12</v>
@@ -5298,12 +5298,12 @@
         <v>6.14</v>
       </c>
       <c r="L83" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B84" s="41">
         <v>1</v>
@@ -5321,7 +5321,7 @@
         <v>19</v>
       </c>
       <c r="G84" s="47" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H84" s="41" t="s">
         <v>12</v>
@@ -5335,12 +5335,12 @@
         <v>4.95</v>
       </c>
       <c r="L84" s="41" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B85" s="41">
         <v>1</v>
@@ -5358,7 +5358,7 @@
         <v>19</v>
       </c>
       <c r="G85" s="47" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H85" s="41" t="s">
         <v>12</v>
@@ -5372,12 +5372,12 @@
         <v>4.95</v>
       </c>
       <c r="L85" s="41" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B86" s="41">
         <v>1</v>
@@ -5395,7 +5395,7 @@
         <v>19</v>
       </c>
       <c r="G86" s="47" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H86" s="41" t="s">
         <v>12</v>
@@ -5409,13 +5409,13 @@
         <v>4.95</v>
       </c>
       <c r="L86" s="41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M86" s="15"/>
     </row>
     <row r="87" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B87" s="41">
         <v>1</v>
@@ -5433,7 +5433,7 @@
         <v>19</v>
       </c>
       <c r="G87" s="47" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H87" s="41" t="s">
         <v>12</v>
@@ -5447,12 +5447,12 @@
         <v>4.95</v>
       </c>
       <c r="L87" s="41" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="76" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B88" s="41">
         <v>10</v>
@@ -5468,7 +5468,7 @@
       </c>
       <c r="F88" s="41"/>
       <c r="G88" s="106" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H88" s="41" t="s">
         <v>12</v>
@@ -5482,12 +5482,12 @@
         <v>3.67</v>
       </c>
       <c r="L88" s="77" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="78" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B89" s="72">
         <v>10</v>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="F89" s="72"/>
       <c r="G89" s="107" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H89" s="72" t="s">
         <v>12</v>
@@ -5517,12 +5517,12 @@
         <v>0.4</v>
       </c>
       <c r="L89" s="80" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="81" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B90" s="82">
         <v>0</v>
@@ -5550,12 +5550,12 @@
         <v>0</v>
       </c>
       <c r="L90" s="82" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="81" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B91" s="82">
         <v>0</v>
@@ -5583,12 +5583,12 @@
         <v>0</v>
       </c>
       <c r="L91" s="86" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="87" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B92" s="72">
         <v>1</v>
@@ -5604,7 +5604,7 @@
       </c>
       <c r="F92" s="72"/>
       <c r="G92" s="88" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H92" s="72" t="s">
         <v>12</v>
@@ -5618,12 +5618,12 @@
         <v>7.99</v>
       </c>
       <c r="L92" s="89" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="87" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B93" s="72">
         <v>1</v>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="F93" s="72"/>
       <c r="G93" s="88" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H93" s="72" t="s">
         <v>12</v>
@@ -5653,12 +5653,12 @@
         <v>15.59</v>
       </c>
       <c r="L93" s="89" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="87" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B94" s="72">
         <v>1</v>
@@ -5674,7 +5674,7 @@
       </c>
       <c r="F94" s="72"/>
       <c r="G94" s="88" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H94" s="72" t="s">
         <v>12</v>
@@ -5688,12 +5688,12 @@
         <v>12.56</v>
       </c>
       <c r="L94" s="90" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="87" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B95" s="72">
         <v>1</v>
@@ -5709,7 +5709,7 @@
       </c>
       <c r="F95" s="72"/>
       <c r="G95" s="88" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H95" s="72" t="s">
         <v>12</v>
@@ -5723,12 +5723,12 @@
         <v>15.59</v>
       </c>
       <c r="L95" s="89" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="87" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B96" s="72">
         <v>1</v>
@@ -5744,7 +5744,7 @@
       </c>
       <c r="F96" s="72"/>
       <c r="G96" s="88" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H96" s="72" t="s">
         <v>12</v>
@@ -5758,7 +5758,7 @@
         <v>15.59</v>
       </c>
       <c r="L96" s="89" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5779,7 +5779,7 @@
       </c>
       <c r="F97" s="63"/>
       <c r="G97" s="68" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H97" s="63" t="s">
         <v>12</v>
@@ -5793,7 +5793,7 @@
         <v>19.75</v>
       </c>
       <c r="L97" s="69" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5975,7 +5975,7 @@
     </row>
     <row r="103" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="31" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B103" s="42">
         <v>25</v>
@@ -5990,16 +5990,16 @@
         <v>90</v>
       </c>
       <c r="F103" s="42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G103" s="108" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H103" s="49" t="s">
         <v>93</v>
       </c>
       <c r="I103" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J103" s="33">
         <v>3.78</v>
@@ -6009,12 +6009,12 @@
         <v>3.78</v>
       </c>
       <c r="L103" s="103" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B104" s="42">
         <v>4</v>
@@ -6029,16 +6029,16 @@
         <v>90</v>
       </c>
       <c r="F104" s="42" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G104" s="50" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H104" s="51" t="s">
         <v>93</v>
       </c>
       <c r="I104" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J104" s="33">
         <v>0.96</v>
@@ -6048,12 +6048,12 @@
         <v>3.84</v>
       </c>
       <c r="L104" s="103" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="35" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="34" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B105" s="42">
         <v>1</v>
@@ -6065,10 +6065,10 @@
         <v>1</v>
       </c>
       <c r="E105" s="42" t="s">
+        <v>340</v>
+      </c>
+      <c r="F105" s="42" t="s">
         <v>341</v>
-      </c>
-      <c r="F105" s="42" t="s">
-        <v>342</v>
       </c>
       <c r="G105" s="104"/>
       <c r="H105" s="51" t="s">
@@ -6083,12 +6083,12 @@
         <v>11.75</v>
       </c>
       <c r="L105" s="103" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="106" spans="1:12" s="35" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="34" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B106" s="42">
         <v>1</v>
@@ -6100,10 +6100,10 @@
         <v>1</v>
       </c>
       <c r="E106" s="42" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F106" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G106" s="104"/>
       <c r="H106" s="51" t="s">
@@ -6118,7 +6118,7 @@
         <v>15.25</v>
       </c>
       <c r="L106" s="103" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6149,7 +6149,7 @@
       <c r="C109" s="17"/>
       <c r="D109" s="18"/>
       <c r="E109" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F109" s="20">
         <v>10</v>
@@ -6166,7 +6166,7 @@
       <c r="C110" s="17"/>
       <c r="D110" s="18"/>
       <c r="E110" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F110" s="20">
         <v>10</v>
@@ -15660,7 +15660,7 @@
     <hyperlink ref="L21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="L22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="L26" r:id="rId15" location="90631A007" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="L37" r:id="rId16" location="368=229" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="L37" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="L38" r:id="rId17" location="48925k93/=18nja2z" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="L44" r:id="rId18" location="95947A007" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="L46" r:id="rId19" location="92141A005" xr:uid="{00000000-0004-0000-0000-000012000000}"/>

</xml_diff>

<commit_message>
Description for 'C2003B-50-ND' and 'C2015R-50-ND' should be '24AWG' and not '30AWG'
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cox/Documents/open source rover/osr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Desktop/fork/open-source-rover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ECEBFA-672B-4342-96F7-6ECD47783B6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54E9ECE-428B-A34D-93CD-4ED4A178D56A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57180" yWindow="2360" windowWidth="33600" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -799,18 +799,12 @@
     <t>E7</t>
   </si>
   <si>
-    <t>Black Wire 30AWG</t>
-  </si>
-  <si>
     <t>C2003B-50-ND</t>
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/general-cable-carol-brand/C2003A.11.01/C2003B-50-ND/5226402</t>
   </si>
   <si>
-    <t>Red Wire 30AWG</t>
-  </si>
-  <si>
     <t>C2015R-50-ND</t>
   </si>
   <si>
@@ -1118,6 +1112,12 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/6157k14</t>
+  </si>
+  <si>
+    <t>Red Wire 24AWG</t>
+  </si>
+  <si>
+    <t>Black Wire 24AWG</t>
   </si>
 </sst>
 </file>
@@ -2010,8 +2010,8 @@
   <dimension ref="A1:AA970"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
+      <pane ySplit="4" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2035,7 +2035,7 @@
   <sheetData>
     <row r="1" spans="1:27" s="109" customFormat="1" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="123" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B1" s="124"/>
       <c r="C1" s="124"/>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="2" spans="1:27" s="111" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="127" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B2" s="127"/>
       <c r="C2" s="127"/>
@@ -2062,7 +2062,7 @@
       <c r="H2" s="114"/>
       <c r="I2" s="114"/>
       <c r="J2" s="119" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K2" s="120">
         <f>SUM(K5:K150)</f>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="3" spans="1:27" s="111" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="115" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B3" s="115"/>
       <c r="C3" s="115"/>
@@ -2110,7 +2110,7 @@
         <v>6</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>7</v>
@@ -2445,7 +2445,7 @@
         <v>58</v>
       </c>
       <c r="I12" s="61" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J12" s="23">
         <v>9.25</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="17" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B17" s="39">
         <v>25</v>
@@ -2634,7 +2634,7 @@
         <v>74</v>
       </c>
       <c r="G17" s="116" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H17" s="39" t="s">
         <v>12</v>
@@ -2648,13 +2648,13 @@
         <v>0.72</v>
       </c>
       <c r="L17" s="117" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B18" s="39">
         <v>25</v>
@@ -2672,7 +2672,7 @@
         <v>53</v>
       </c>
       <c r="G18" s="116" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H18" s="39" t="s">
         <v>12</v>
@@ -2686,7 +2686,7 @@
         <v>0.72</v>
       </c>
       <c r="L18" s="110" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M18" s="9"/>
     </row>
@@ -2762,7 +2762,7 @@
         <v>4.49</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M20" s="9"/>
     </row>
@@ -2792,7 +2792,7 @@
         <v>58</v>
       </c>
       <c r="I21" s="61" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J21" s="23">
         <v>25.27</v>
@@ -2832,7 +2832,7 @@
         <v>58</v>
       </c>
       <c r="I22" s="61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J22" s="23">
         <v>12.9</v>
@@ -2872,7 +2872,7 @@
         <v>58</v>
       </c>
       <c r="I23" s="61" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J23" s="23">
         <f>38.9+36.9</f>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="24" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B24" s="39">
         <v>300</v>
@@ -2914,7 +2914,7 @@
         <v>93</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J24" s="23">
         <v>3.45</v>
@@ -2954,7 +2954,7 @@
         <v>93</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J25" s="23">
         <v>5.61</v>
@@ -2998,7 +2998,7 @@
         <v>93</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J26" s="23">
         <v>2.72</v>
@@ -3041,7 +3041,7 @@
         <v>93</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J27" s="23">
         <v>2.79</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="28" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B28" s="39">
         <v>100</v>
@@ -3085,7 +3085,7 @@
         <v>93</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J28" s="23">
         <v>3.72</v>
@@ -3095,7 +3095,7 @@
         <v>3.72</v>
       </c>
       <c r="L28" s="27" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="M28" s="9"/>
       <c r="Y28" s="9"/>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B29" s="39">
         <v>100</v>
@@ -3128,7 +3128,7 @@
         <v>93</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J29" s="23">
         <v>3.72</v>
@@ -3138,7 +3138,7 @@
         <v>3.72</v>
       </c>
       <c r="L29" s="27" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M29" s="9"/>
       <c r="Y29" s="9"/>
@@ -3147,7 +3147,7 @@
     </row>
     <row r="30" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B30" s="41">
         <v>100</v>
@@ -3171,7 +3171,7 @@
         <v>93</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J30" s="23">
         <v>4.07</v>
@@ -3181,13 +3181,13 @@
         <v>4.07</v>
       </c>
       <c r="L30" s="26" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B31" s="41">
         <v>100</v>
@@ -3211,7 +3211,7 @@
         <v>93</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J31" s="23">
         <v>4.41</v>
@@ -3221,13 +3221,13 @@
         <v>4.41</v>
       </c>
       <c r="L31" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="M31" s="9"/>
     </row>
     <row r="32" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B32" s="41">
         <v>50</v>
@@ -3251,7 +3251,7 @@
         <v>93</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J32" s="23">
         <v>5.42</v>
@@ -3261,13 +3261,13 @@
         <v>5.42</v>
       </c>
       <c r="L32" s="26" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M32" s="9"/>
     </row>
     <row r="33" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B33" s="39">
         <v>50</v>
@@ -3291,7 +3291,7 @@
         <v>93</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J33" s="23">
         <v>6.51</v>
@@ -3301,13 +3301,13 @@
         <v>6.51</v>
       </c>
       <c r="L33" s="27" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="M33" s="9"/>
     </row>
     <row r="34" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B34" s="39">
         <v>100</v>
@@ -3331,7 +3331,7 @@
         <v>93</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J34" s="23">
         <v>2.87</v>
@@ -3347,7 +3347,7 @@
     </row>
     <row r="35" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B35" s="41">
         <v>100</v>
@@ -3371,7 +3371,7 @@
         <v>93</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J35" s="23">
         <v>7.7</v>
@@ -3381,7 +3381,7 @@
         <v>7.7</v>
       </c>
       <c r="L35" s="26" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -3405,13 +3405,13 @@
         <v>126</v>
       </c>
       <c r="G36" s="43" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H36" s="39" t="s">
         <v>58</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J36" s="23">
         <v>23.16</v>
@@ -3421,7 +3421,7 @@
         <v>23.16</v>
       </c>
       <c r="L36" s="110" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -3451,7 +3451,7 @@
         <v>58</v>
       </c>
       <c r="I37" s="61" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J37" s="23">
         <v>2.72</v>
@@ -3461,7 +3461,7 @@
         <v>29.92</v>
       </c>
       <c r="L37" s="110" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="M37" s="9"/>
     </row>
@@ -3491,7 +3491,7 @@
         <v>58</v>
       </c>
       <c r="I38" s="61" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J38" s="23">
         <v>4.92</v>
@@ -3531,7 +3531,7 @@
         <v>93</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J39" s="23">
         <v>0.23</v>
@@ -3571,7 +3571,7 @@
         <v>93</v>
       </c>
       <c r="I40" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J40" s="23">
         <v>0.3</v>
@@ -3612,7 +3612,7 @@
         <v>93</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J41" s="23">
         <v>0.23</v>
@@ -3652,7 +3652,7 @@
         <v>93</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J42" s="23">
         <v>0.27</v>
@@ -3695,7 +3695,7 @@
         <v>93</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J43" s="23">
         <v>0.37</v>
@@ -3738,7 +3738,7 @@
         <v>93</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J44" s="23">
         <v>0.48</v>
@@ -3781,7 +3781,7 @@
         <v>93</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J45" s="23">
         <v>1.17</v>
@@ -3824,7 +3824,7 @@
         <v>93</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J46" s="23">
         <v>1.4</v>
@@ -3864,7 +3864,7 @@
         <v>93</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J47" s="23">
         <v>2.4700000000000002</v>
@@ -3956,7 +3956,7 @@
     </row>
     <row r="50" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B50" s="39">
         <v>6</v>
@@ -3988,7 +3988,7 @@
         <v>209.70000000000002</v>
       </c>
       <c r="L50" s="110" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M50" s="9">
         <v>0</v>
@@ -4028,7 +4028,7 @@
         <v>79.8</v>
       </c>
       <c r="L51" s="110" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M51" s="9"/>
     </row>
@@ -4058,7 +4058,7 @@
         <v>58</v>
       </c>
       <c r="I52" s="61" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J52" s="23">
         <v>2.99</v>
@@ -4098,7 +4098,7 @@
         <v>58</v>
       </c>
       <c r="I53" s="61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J53" s="23">
         <v>5.99</v>
@@ -4138,7 +4138,7 @@
         <v>58</v>
       </c>
       <c r="I54" s="61" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J54" s="23">
         <v>6.99</v>
@@ -4178,7 +4178,7 @@
         <v>58</v>
       </c>
       <c r="I55" s="61" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J55" s="23">
         <v>5.99</v>
@@ -4218,7 +4218,7 @@
         <v>58</v>
       </c>
       <c r="I56" s="61" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J56" s="23">
         <v>5.99</v>
@@ -4258,7 +4258,7 @@
         <v>58</v>
       </c>
       <c r="I57" s="61" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J57" s="23">
         <v>5.99</v>
@@ -4298,7 +4298,7 @@
         <v>58</v>
       </c>
       <c r="I58" s="61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J58" s="23">
         <v>1.49</v>
@@ -4338,7 +4338,7 @@
         <v>58</v>
       </c>
       <c r="I59" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J59" s="23">
         <v>5.99</v>
@@ -4378,7 +4378,7 @@
         <v>58</v>
       </c>
       <c r="I60" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J60" s="23">
         <v>2.09</v>
@@ -4418,7 +4418,7 @@
         <v>58</v>
       </c>
       <c r="I61" s="25" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J61" s="23">
         <v>1.49</v>
@@ -4458,7 +4458,7 @@
         <v>58</v>
       </c>
       <c r="I62" s="61" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J62" s="23">
         <v>3.99</v>
@@ -4498,7 +4498,7 @@
         <v>58</v>
       </c>
       <c r="I63" s="61" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J63" s="23">
         <v>5.99</v>
@@ -4538,7 +4538,7 @@
         <v>58</v>
       </c>
       <c r="I64" s="61" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J64" s="23">
         <v>2.39</v>
@@ -4578,7 +4578,7 @@
         <v>58</v>
       </c>
       <c r="I65" s="61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J65" s="23">
         <v>4.99</v>
@@ -4618,7 +4618,7 @@
         <v>58</v>
       </c>
       <c r="I66" s="61" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J66" s="23">
         <v>9.99</v>
@@ -4658,7 +4658,7 @@
         <v>58</v>
       </c>
       <c r="I67" s="61" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J67" s="23">
         <v>5.99</v>
@@ -4698,7 +4698,7 @@
         <v>58</v>
       </c>
       <c r="I68" s="61" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J68" s="23">
         <v>3.69</v>
@@ -4738,7 +4738,7 @@
         <v>58</v>
       </c>
       <c r="I69" s="61" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J69" s="23">
         <v>7.99</v>
@@ -4778,7 +4778,7 @@
         <v>58</v>
       </c>
       <c r="I70" s="61" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J70" s="23">
         <v>4.49</v>
@@ -4818,7 +4818,7 @@
         <v>58</v>
       </c>
       <c r="I71" s="61" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J71" s="23">
         <v>16.989999999999998</v>
@@ -4858,7 +4858,7 @@
         <v>58</v>
       </c>
       <c r="I72" s="61" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J72" s="23">
         <v>13.99</v>
@@ -4898,7 +4898,7 @@
         <v>58</v>
       </c>
       <c r="I73" s="73" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J73" s="23">
         <v>4.99</v>
@@ -4938,7 +4938,7 @@
         <v>58</v>
       </c>
       <c r="I74" s="61" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J74" s="23">
         <v>7.99</v>
@@ -4979,7 +4979,7 @@
         <v>58</v>
       </c>
       <c r="I75" s="61" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J75" s="23">
         <v>3.99</v>
@@ -5019,7 +5019,7 @@
         <v>58</v>
       </c>
       <c r="I76" s="61" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J76" s="23">
         <v>2.79</v>
@@ -5059,7 +5059,7 @@
         <v>58</v>
       </c>
       <c r="I77" s="61" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J77" s="23">
         <v>1.29</v>
@@ -5099,7 +5099,7 @@
         <v>58</v>
       </c>
       <c r="I78" s="25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J78" s="23">
         <v>3.99</v>
@@ -5139,7 +5139,7 @@
         <v>93</v>
       </c>
       <c r="I79" s="25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J79" s="23">
         <v>1.79</v>
@@ -5172,7 +5172,7 @@
         <v>255</v>
       </c>
       <c r="G80" s="43" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H80" s="60" t="s">
         <v>12</v>
@@ -5209,7 +5209,7 @@
         <v>257</v>
       </c>
       <c r="G81" s="43" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H81" s="60" t="s">
         <v>12</v>
@@ -5228,7 +5228,7 @@
     </row>
     <row r="82" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="21" t="s">
-        <v>258</v>
+        <v>364</v>
       </c>
       <c r="B82" s="41">
         <v>1</v>
@@ -5246,7 +5246,7 @@
         <v>19</v>
       </c>
       <c r="G82" s="47" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H82" s="41" t="s">
         <v>12</v>
@@ -5260,13 +5260,13 @@
         <v>6.32</v>
       </c>
       <c r="L82" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M82" s="15"/>
     </row>
     <row r="83" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="21" t="s">
-        <v>261</v>
+        <v>363</v>
       </c>
       <c r="B83" s="41">
         <v>1</v>
@@ -5284,7 +5284,7 @@
         <v>19</v>
       </c>
       <c r="G83" s="43" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H83" s="41" t="s">
         <v>12</v>
@@ -5298,12 +5298,12 @@
         <v>6.14</v>
       </c>
       <c r="L83" s="30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="21" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B84" s="41">
         <v>1</v>
@@ -5321,7 +5321,7 @@
         <v>19</v>
       </c>
       <c r="G84" s="47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H84" s="41" t="s">
         <v>12</v>
@@ -5335,12 +5335,12 @@
         <v>4.95</v>
       </c>
       <c r="L84" s="41" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B85" s="41">
         <v>1</v>
@@ -5358,7 +5358,7 @@
         <v>19</v>
       </c>
       <c r="G85" s="47" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H85" s="41" t="s">
         <v>12</v>
@@ -5372,12 +5372,12 @@
         <v>4.95</v>
       </c>
       <c r="L85" s="41" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B86" s="41">
         <v>1</v>
@@ -5395,7 +5395,7 @@
         <v>19</v>
       </c>
       <c r="G86" s="47" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H86" s="41" t="s">
         <v>12</v>
@@ -5409,13 +5409,13 @@
         <v>4.95</v>
       </c>
       <c r="L86" s="41" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M86" s="15"/>
     </row>
     <row r="87" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B87" s="41">
         <v>1</v>
@@ -5433,7 +5433,7 @@
         <v>19</v>
       </c>
       <c r="G87" s="47" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H87" s="41" t="s">
         <v>12</v>
@@ -5447,12 +5447,12 @@
         <v>4.95</v>
       </c>
       <c r="L87" s="41" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="76" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B88" s="41">
         <v>10</v>
@@ -5468,7 +5468,7 @@
       </c>
       <c r="F88" s="41"/>
       <c r="G88" s="106" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H88" s="41" t="s">
         <v>12</v>
@@ -5482,12 +5482,12 @@
         <v>3.67</v>
       </c>
       <c r="L88" s="77" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="78" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B89" s="72">
         <v>10</v>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="F89" s="72"/>
       <c r="G89" s="107" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H89" s="72" t="s">
         <v>12</v>
@@ -5517,12 +5517,12 @@
         <v>0.4</v>
       </c>
       <c r="L89" s="80" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="81" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B90" s="82">
         <v>0</v>
@@ -5550,12 +5550,12 @@
         <v>0</v>
       </c>
       <c r="L90" s="82" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="81" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B91" s="82">
         <v>0</v>
@@ -5583,12 +5583,12 @@
         <v>0</v>
       </c>
       <c r="L91" s="86" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="87" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B92" s="72">
         <v>1</v>
@@ -5604,7 +5604,7 @@
       </c>
       <c r="F92" s="72"/>
       <c r="G92" s="88" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H92" s="72" t="s">
         <v>12</v>
@@ -5618,12 +5618,12 @@
         <v>7.99</v>
       </c>
       <c r="L92" s="89" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="87" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B93" s="72">
         <v>1</v>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="F93" s="72"/>
       <c r="G93" s="88" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H93" s="72" t="s">
         <v>12</v>
@@ -5653,12 +5653,12 @@
         <v>15.59</v>
       </c>
       <c r="L93" s="89" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="87" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B94" s="72">
         <v>1</v>
@@ -5674,7 +5674,7 @@
       </c>
       <c r="F94" s="72"/>
       <c r="G94" s="88" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H94" s="72" t="s">
         <v>12</v>
@@ -5688,12 +5688,12 @@
         <v>12.56</v>
       </c>
       <c r="L94" s="90" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="87" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B95" s="72">
         <v>1</v>
@@ -5709,7 +5709,7 @@
       </c>
       <c r="F95" s="72"/>
       <c r="G95" s="88" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H95" s="72" t="s">
         <v>12</v>
@@ -5723,12 +5723,12 @@
         <v>15.59</v>
       </c>
       <c r="L95" s="89" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="87" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B96" s="72">
         <v>1</v>
@@ -5744,7 +5744,7 @@
       </c>
       <c r="F96" s="72"/>
       <c r="G96" s="88" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H96" s="72" t="s">
         <v>12</v>
@@ -5758,7 +5758,7 @@
         <v>15.59</v>
       </c>
       <c r="L96" s="89" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="97" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5779,7 +5779,7 @@
       </c>
       <c r="F97" s="63"/>
       <c r="G97" s="68" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H97" s="63" t="s">
         <v>12</v>
@@ -5793,7 +5793,7 @@
         <v>19.75</v>
       </c>
       <c r="L97" s="69" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="98" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5975,7 +5975,7 @@
     </row>
     <row r="103" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="31" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B103" s="42">
         <v>25</v>
@@ -5990,16 +5990,16 @@
         <v>90</v>
       </c>
       <c r="F103" s="42" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G103" s="108" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="H103" s="49" t="s">
         <v>93</v>
       </c>
       <c r="I103" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J103" s="33">
         <v>3.78</v>
@@ -6009,12 +6009,12 @@
         <v>3.78</v>
       </c>
       <c r="L103" s="103" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="34" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B104" s="42">
         <v>4</v>
@@ -6029,16 +6029,16 @@
         <v>90</v>
       </c>
       <c r="F104" s="42" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G104" s="50" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H104" s="51" t="s">
         <v>93</v>
       </c>
       <c r="I104" s="32" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J104" s="33">
         <v>0.96</v>
@@ -6048,12 +6048,12 @@
         <v>3.84</v>
       </c>
       <c r="L104" s="103" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="35" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="34" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B105" s="42">
         <v>1</v>
@@ -6065,10 +6065,10 @@
         <v>1</v>
       </c>
       <c r="E105" s="42" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F105" s="42" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G105" s="104"/>
       <c r="H105" s="51" t="s">
@@ -6083,12 +6083,12 @@
         <v>11.75</v>
       </c>
       <c r="L105" s="103" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="106" spans="1:12" s="35" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="34" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B106" s="42">
         <v>1</v>
@@ -6100,7 +6100,7 @@
         <v>1</v>
       </c>
       <c r="E106" s="42" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F106" s="42" t="s">
         <v>169</v>
@@ -6118,7 +6118,7 @@
         <v>15.25</v>
       </c>
       <c r="L106" s="103" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6149,7 +6149,7 @@
       <c r="C109" s="17"/>
       <c r="D109" s="18"/>
       <c r="E109" s="20" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F109" s="20">
         <v>10</v>
@@ -6166,7 +6166,7 @@
       <c r="C110" s="17"/>
       <c r="D110" s="18"/>
       <c r="E110" s="20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F110" s="20">
         <v>10</v>

</xml_diff>

<commit_message>
4.5 inch channel had wrong link in Column L
</commit_message>
<xml_diff>
--- a/osr_Master_parts_list.xlsx
+++ b/osr_Master_parts_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cox/Documents/open source rover/osr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Desktop/fork/open-source-rover/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97ECEBFA-672B-4342-96F7-6ECD47783B6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1247A89-427C-6F4B-B4EE-0B5AD6967518}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57180" yWindow="2360" windowWidth="33600" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="366">
   <si>
     <t>Part</t>
   </si>
@@ -1118,6 +1118,9 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/6157k14</t>
+  </si>
+  <si>
+    <t>4.50” Aluminum Channel</t>
   </si>
 </sst>
 </file>
@@ -2009,9 +2012,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA970"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4907,8 +4910,8 @@
         <f t="shared" si="2"/>
         <v>19.96</v>
       </c>
-      <c r="L73" s="28" t="s">
-        <v>234</v>
+      <c r="L73" s="110" t="s">
+        <v>365</v>
       </c>
       <c r="M73" s="9"/>
     </row>
@@ -15708,29 +15711,29 @@
     <hyperlink ref="L100" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
     <hyperlink ref="L101" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
     <hyperlink ref="L102" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="L73" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="L24" r:id="rId65" location="92949a144/=18njs1n" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="L30" r:id="rId66" location="92949A150" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="L34" r:id="rId67" location="92949a106/=18njrx6" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="L104" r:id="rId68" location="93330A252" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="L27" r:id="rId69" location="90631A005" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="L28" r:id="rId70" location="92949A146" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="L29" r:id="rId71" location="92949A148" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="L31" r:id="rId72" location="92949A151" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="L32" r:id="rId73" location="92949A153" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="L33" r:id="rId74" location="92949A160" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="L39" r:id="rId75" location="92510A442" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="L41" r:id="rId76" location="91780A162" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="L42" r:id="rId77" location="91780A164" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="L43" r:id="rId78" location="91780A166" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="L47" r:id="rId79" location="91545A280" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="L45" r:id="rId80" location="92141A008" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="L105" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="L106" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="L91" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="L17" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="L18" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="L50" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="L24" r:id="rId64" location="92949a144/=18njs1n" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="L30" r:id="rId65" location="92949A150" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="L34" r:id="rId66" location="92949a106/=18njrx6" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="L104" r:id="rId67" location="93330A252" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="L27" r:id="rId68" location="90631A005" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="L28" r:id="rId69" location="92949A146" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="L29" r:id="rId70" location="92949A148" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="L31" r:id="rId71" location="92949A151" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="L32" r:id="rId72" location="92949A153" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="L33" r:id="rId73" location="92949A160" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="L39" r:id="rId74" location="92510A442" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="L41" r:id="rId75" location="91780A162" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="L42" r:id="rId76" location="91780A164" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="L43" r:id="rId77" location="91780A166" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="L47" r:id="rId78" location="91545A280" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="L45" r:id="rId79" location="92141A008" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="L105" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="L106" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="L91" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="L17" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="L18" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="L50" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="L73" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId87"/>

</xml_diff>